<commit_message>
Rearranged LBCB Operation Manager.vi displays. Added set target button
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>The input file should start from the beginning.</t>
+  </si>
+  <si>
+    <t>Press Pause</t>
+  </si>
+  <si>
+    <t>Test execution should continue from the current target.</t>
   </si>
 </sst>
 </file>
@@ -668,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,6 +1217,22 @@
       </c>
       <c r="C51" s="1" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing.  New configuration for two box crane bay.
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -141,9 +141,6 @@
     <t>Multiple targets are executed until a target exceeds a limit and a fault is generated.  The fault light should become red and a message indicating the DOF that has faulted should be displayed.  Pause/Running should be paused.</t>
   </si>
   <si>
-    <t>Input a target of displacements within the displacement limits</t>
-  </si>
-  <si>
     <t>Input a ramp time of 10 seconds</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Press stop during the hold state</t>
   </si>
   <si>
-    <t>Input a target of displacements where one DOF is set beyond the limit.</t>
-  </si>
-  <si>
     <t>Press start</t>
   </si>
   <si>
@@ -177,33 +171,21 @@
     <t>Repeat these steps with other DOFs.</t>
   </si>
   <si>
-    <t>Input a target of displacements that are less than half way to the displacement limits.</t>
-  </si>
-  <si>
     <t>Open the Offsets window and set offsets for both command and measured displacements.  Press OK to exit the window</t>
   </si>
   <si>
     <t>Click on the 'Global' button to switch it to 'Local'</t>
   </si>
   <si>
-    <t>Enter another target that is a small increment past zero</t>
-  </si>
-  <si>
     <t>Press the start button</t>
   </si>
   <si>
     <t>Switch from Local to Global</t>
   </si>
   <si>
-    <t>Enter a target that is a small increment past the current position.</t>
-  </si>
-  <si>
     <t>Switch from Global to Local</t>
   </si>
   <si>
-    <t>Open the limits display and check the Local limit for a DOF.  Record the global limit also.  Close the limits display and set a target that is just beyond the local limit</t>
-  </si>
-  <si>
     <t>Clear the fault by extending the limit.  Switch from Global to Local</t>
   </si>
   <si>
@@ -253,6 +235,24 @@
   </si>
   <si>
     <t>Test execution should continue from the current target.</t>
+  </si>
+  <si>
+    <t>Input a target of displacements within the displacement limits and press "Set Target"</t>
+  </si>
+  <si>
+    <t>Input a target of displacements where one DOF is set beyond the limit and press "Set Target".</t>
+  </si>
+  <si>
+    <t>Input a target of displacements that are less than half way to the displacement limits and press "Set Target".</t>
+  </si>
+  <si>
+    <t>Enter another target that is a small increment past zero and press "Set Target"</t>
+  </si>
+  <si>
+    <t>Enter a target that is a small increment past the current position and press "Set Target".</t>
+  </si>
+  <si>
+    <t>Open the limits display and check the Local limit for a DOF.  Record the global limit also.  Close the limits display and set a target that is just beyond the local limit and press "Set Target".</t>
   </si>
 </sst>
 </file>
@@ -674,10 +674,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,12 +709,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -722,7 +725,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -731,7 +734,7 @@
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
@@ -742,7 +745,7 @@
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -753,7 +756,7 @@
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
@@ -761,12 +764,12 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -777,7 +780,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -786,7 +789,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
@@ -797,7 +800,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>11</v>
@@ -808,7 +811,7 @@
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -819,7 +822,7 @@
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -830,7 +833,7 @@
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>5</v>
@@ -841,7 +844,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>12</v>
@@ -852,7 +855,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
@@ -865,7 +868,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -876,7 +879,7 @@
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>15</v>
@@ -887,7 +890,7 @@
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>16</v>
@@ -898,7 +901,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>17</v>
@@ -911,7 +914,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -922,7 +925,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
@@ -931,7 +934,7 @@
     <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>20</v>
@@ -942,7 +945,7 @@
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="5"/>
@@ -951,7 +954,7 @@
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>19</v>
@@ -959,10 +962,10 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -973,7 +976,7 @@
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>21</v>
@@ -984,7 +987,7 @@
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>22</v>
@@ -995,7 +998,7 @@
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -1006,7 +1009,7 @@
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>23</v>
@@ -1017,7 +1020,7 @@
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>24</v>
@@ -1028,7 +1031,7 @@
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="4" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1039,7 +1042,7 @@
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>25</v>
@@ -1050,7 +1053,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>26</v>
@@ -1061,7 +1064,7 @@
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>16</v>
@@ -1072,7 +1075,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>27</v>
@@ -1083,7 +1086,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>28</v>
@@ -1094,7 +1097,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>29</v>
@@ -1107,7 +1110,7 @@
         <v>32</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>33</v>
@@ -1117,7 +1120,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>33</v>
@@ -1125,7 +1128,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>34</v>
@@ -1133,7 +1136,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>35</v>
@@ -1141,7 +1144,7 @@
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>36</v>
@@ -1149,7 +1152,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>37</v>
@@ -1157,7 +1160,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>34</v>
@@ -1165,7 +1168,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>27</v>
@@ -1173,7 +1176,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>38</v>
@@ -1181,7 +1184,7 @@
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>39</v>
@@ -1189,7 +1192,7 @@
     </row>
     <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>40</v>
@@ -1197,7 +1200,7 @@
     </row>
     <row r="49" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>16</v>
@@ -1205,23 +1208,23 @@
     </row>
     <row r="50" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>33</v>
@@ -1229,10 +1232,10 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1242,7 +1245,7 @@
     <mergeCell ref="A20:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MM refactoring fake daq testing
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370"/>
   </bookViews>
   <sheets>
-    <sheet name="Displacement Tests" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Startup" sheetId="2" r:id="rId1"/>
+    <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -253,6 +253,51 @@
   </si>
   <si>
     <t>Open the limits display and check the Local limit for a DOF.  Record the global limit also.  Close the limits display and set a target that is just beyond the local limit and press "Set Target".</t>
+  </si>
+  <si>
+    <t>Fake Startup</t>
+  </si>
+  <si>
+    <t>Double click on the file "LBCB Operation Manager Project.lvproj"</t>
+  </si>
+  <si>
+    <t>LabVIEW should start up and display the project tree</t>
+  </si>
+  <si>
+    <t>Double click on "LBCB Operations Manager.vi" and "Mixed Mode Widget.vi"</t>
+  </si>
+  <si>
+    <t>Both vi's should open with a clean arrow</t>
+  </si>
+  <si>
+    <t>Press the blue Real button</t>
+  </si>
+  <si>
+    <t>The button should turn pink and say Fake</t>
+  </si>
+  <si>
+    <t>Press Start Autobalancing on the LBCB Operation Manager</t>
+  </si>
+  <si>
+    <t>Press the start arrow on the LBCB Operation Manager and then the Mixed Mode Widget</t>
+  </si>
+  <si>
+    <t>The auto balance initialization and Command Displacement Difference window should appear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select autobalance on all auto balance windows that appear.  </t>
+  </si>
+  <si>
+    <t>Both widgets should be running.  The Mixed Mode target and input mode window should be grayed out.</t>
+  </si>
+  <si>
+    <t>A warning popup should show up.  After ok'ing the popup, the system should start autobalancing.  After it is balanced there will most likely be numerous limit faults because the fake initial position is deliberately skewed.  The limits will need to be adjusted to correct these faults before any further testing is done.</t>
+  </si>
+  <si>
+    <t>Press control on one or both LBCBs</t>
+  </si>
+  <si>
+    <t>The Mixed Mode Widget should now allow inputs</t>
   </si>
 </sst>
 </file>
@@ -284,7 +329,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -344,11 +389,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -371,6 +425,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,13 +734,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,18 +1414,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
MM refactoring fake daq testing Manual mode passed testing
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
     <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Configuration Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="118">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -69,9 +69,6 @@
     <t>The fault light should turn green.  The fault message should clear.  The command for the faulted DOF should not change significantly.</t>
   </si>
   <si>
-    <t>Results should be the same.</t>
-  </si>
-  <si>
     <t>Manual Input Global/Local toggles</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Press stop while the MM State is at 'Ramping'</t>
   </si>
   <si>
-    <t>Type a zero at one of the DOFs and click away.  Do not change the value of the target</t>
-  </si>
-  <si>
     <t>Press Start</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>Open the limits display and extend the limit so that the fault is cleared.</t>
   </si>
   <si>
-    <t>Repeat these steps with other DOFs.</t>
-  </si>
-  <si>
     <t>Open the Offsets window and set offsets for both command and measured displacements.  Press OK to exit the window</t>
   </si>
   <si>
@@ -237,15 +228,6 @@
     <t>Test execution should continue from the current target.</t>
   </si>
   <si>
-    <t>Input a target of displacements within the displacement limits and press "Set Target"</t>
-  </si>
-  <si>
-    <t>Input a target of displacements where one DOF is set beyond the limit and press "Set Target".</t>
-  </si>
-  <si>
-    <t>Input a target of displacements that are less than half way to the displacement limits and press "Set Target".</t>
-  </si>
-  <si>
     <t>Enter another target that is a small increment past zero and press "Set Target"</t>
   </si>
   <si>
@@ -298,6 +280,96 @@
   </si>
   <si>
     <t>The Mixed Mode Widget should now allow inputs</t>
+  </si>
+  <si>
+    <t>Input a target of displacement Dx within the displacement limits and press "Set Target"</t>
+  </si>
+  <si>
+    <t>Repeat test for Dy</t>
+  </si>
+  <si>
+    <t>Repeat test for Dz</t>
+  </si>
+  <si>
+    <t>Repeat test for Rx</t>
+  </si>
+  <si>
+    <t>Repeat test for Ry</t>
+  </si>
+  <si>
+    <t>Repeat test for Rz</t>
+  </si>
+  <si>
+    <t>Repeat test for multiple DOFs and the other LBCB if available</t>
+  </si>
+  <si>
+    <t>Input a target of displacement Dx that is less than half way to the displacement limits and press "Set Target".</t>
+  </si>
+  <si>
+    <t>Repeat test using the actuator displacement limits for all six actuators</t>
+  </si>
+  <si>
+    <t>Input a target displacement for Dx beyond the Dx limit and press "Set Target".</t>
+  </si>
+  <si>
+    <t>Open up the OM Latest Build folder and double click on the "LBCB Operation Manager" executable</t>
+  </si>
+  <si>
+    <t>Two widgets should be running.  For the  Mixed Mode widget, target and input mode window should be grayed out.</t>
+  </si>
+  <si>
+    <t>Real Startup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the difference between command and displacement for all of the actuators and DOFs. </t>
+  </si>
+  <si>
+    <t>The differences should be insignificant.  If they are not the LBCB will jump to its initial position once oil pressure is applied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the small LBCBs turn low pressure on.  </t>
+  </si>
+  <si>
+    <t>Verify that the forces have not changed significantly</t>
+  </si>
+  <si>
+    <t>For the large LBCBs turn low pressure on and unlock the actuators one at a time starting with the Z actuators.</t>
+  </si>
+  <si>
+    <t>Switch to high pressure</t>
+  </si>
+  <si>
+    <t>The forces will jump somewhat but then settle to an equilibrium.  This equilibrium is zero unless the LBCB is connected to a specimen.  If a specimen is connected then the equilbrium will be close to the last position the LBCB was moved to before it was shut down.</t>
+  </si>
+  <si>
+    <t>Real Startup procedure needs to done up to the point where the control for each LBCB is turned on.  Oil pressure should not be used for this test.</t>
+  </si>
+  <si>
+    <t>The Mixed Mode widget should be ready to accept commands.</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeat test for the target patterns "Displacements Only", "Rotations Only", and "Displacements &amp; Rotations" </t>
+  </si>
+  <si>
+    <t>Press Set Target.  Do not change the value of the target</t>
+  </si>
+  <si>
+    <t>Open up the OM Latest Build folder and double click on the "OM Setup" executable</t>
+  </si>
+  <si>
+    <t>OM Setup should display with the Load button blinking</t>
+  </si>
+  <si>
+    <t>OM Setup Test</t>
+  </si>
+  <si>
+    <t>In the OM Latest Build folder,  make a copy of the Config folder so that the configuration can be restored at the end of the test</t>
   </si>
 </sst>
 </file>
@@ -329,7 +401,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -389,20 +461,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -418,6 +481,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -427,10 +493,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -734,9 +800,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -758,79 +824,185 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="1" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="1" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="C12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A7"/>
+  <mergeCells count="2">
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -842,22 +1014,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="58" style="1" customWidth="1"/>
     <col min="3" max="3" width="66.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -868,560 +1041,907 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="F1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="4" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="4"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="6"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="6"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="6"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
       <c r="B23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
       <c r="B25" s="4" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
       <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="6"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="6"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="6"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="6"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="6"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="6"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
       <c r="B34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
       <c r="B36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
       <c r="B38" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+      <c r="B41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+      <c r="B42" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+      <c r="B45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="B48" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="B52" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="B53" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C62" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="C65" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+      <c r="C66" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+      <c r="C67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+      <c r="C68" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
+      <c r="C70" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+      <c r="C71" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A15"/>
-    <mergeCell ref="A20:A37"/>
+  <mergeCells count="5">
+    <mergeCell ref="A57:A72"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A33:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="83.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mixed Mode Refactoring is ready for student testing
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="187">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -186,12 +186,6 @@
     <t>Swtich from Local to Global</t>
   </si>
   <si>
-    <t>Select an input file for each LBCB  being tested that is within the limits of the DOFs being controlled for the first few steps.  Later on in the  test there needs to be a target that exceeds a limit.</t>
-  </si>
-  <si>
-    <t>Press Load</t>
-  </si>
-  <si>
     <t>Press Run</t>
   </si>
   <si>
@@ -427,6 +421,300 @@
   </si>
   <si>
     <t>Repeat the value entry tests for External Sensors</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Clear Targets and press Apply</t>
+  </si>
+  <si>
+    <t>No Targets should be displayed</t>
+  </si>
+  <si>
+    <t>Target Patterns</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Reset to Zero and press Apply</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Displacements Only and press Apply</t>
+  </si>
+  <si>
+    <t>All displacements for all LBCBs should be displayed in the Targets window with their current value</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Displacements &amp; Rotations and press Apply</t>
+  </si>
+  <si>
+    <t>All displacements and rotations for all LBCBs should be displayed in the Targets window with values of zero</t>
+  </si>
+  <si>
+    <t>All displacements and rotations for all LBCBs should be displayed in the Targets window with their current value</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Rotations Only and press Apply</t>
+  </si>
+  <si>
+    <t>All rotations for all LBCBs should be displayed in the Targets window with their current value</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Forces &amp; Moments and press Apply</t>
+  </si>
+  <si>
+    <t>All forces and moments for all LBCBs should be displayed in the Targets window with their current value</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Forces Only and press Apply</t>
+  </si>
+  <si>
+    <t>All forces for all LBCBs should be displayed in the Targets window with their current value</t>
+  </si>
+  <si>
+    <t>Set Target Pattern to Moments Only and press Apply</t>
+  </si>
+  <si>
+    <t>All moments for all LBCBs should be displayed in the Targets window with their current value</t>
+  </si>
+  <si>
+    <t>Press Load and select an input file for each LBCB  being tested that is within the limits of the DOFs being controlled for the first few steps.  Later on in the  test there needs to be a target that exceeds a limit.</t>
+  </si>
+  <si>
+    <t>Select Input File Mode</t>
+  </si>
+  <si>
+    <t>Move the LBCBs to a position close to the nominal origin but not to exactly zero</t>
+  </si>
+  <si>
+    <t>Set the offsets and switch from Global to Local coordinates</t>
+  </si>
+  <si>
+    <t>All of the displacments should read zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch to NTCP mode and press "Connect NTCP" </t>
+  </si>
+  <si>
+    <t>The Socket widget should appear and be running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open up a command window.  Change to the "OM Latest Build" folder located at "C:\Documents and Settings\All Users\Desktop\OM Latest Build"  </t>
+  </si>
+  <si>
+    <t>Type "testNtcpLink.pl --lbcb=?" in the command window where ? Is the number of LBCBs you are controlling</t>
+  </si>
+  <si>
+    <t>The script should start running.  The Mixed Mode window will have a blinking Accept button.  The Targets window will have a target of 1 for the DX of each LBCB.  The test stats window should display step "1 0 4"</t>
+  </si>
+  <si>
+    <t>Press the Accept button</t>
+  </si>
+  <si>
+    <t>The Start button should blink</t>
+  </si>
+  <si>
+    <t>The step should run.  After it is completed the next step is sent from the script.  The Dx should be at -1.  The Accept button should be blinking.</t>
+  </si>
+  <si>
+    <t>Press the Decline button</t>
+  </si>
+  <si>
+    <t>The command window should display "ABORTING PROPOSE COMMAND".  The script should send another step with Dx = 1.  The Accept button should be blinking</t>
+  </si>
+  <si>
+    <t>Press the Accept button and then the Stop button</t>
+  </si>
+  <si>
+    <t>The command window should display "ABORTING EXECUTE COMMAND".  The script should send another step with Dx = -1.  The Accept button should be blinking.</t>
+  </si>
+  <si>
+    <t>Press "Disconnect NTCP" and type &lt;CTRL&gt; C in the command window</t>
+  </si>
+  <si>
+    <t>The Socket widget should disappear.  The Script should stop running.</t>
+  </si>
+  <si>
+    <t>Set the limit for Dx to something more than -1.  Press Accept and then Start</t>
+  </si>
+  <si>
+    <t>The ramp should run until the limit is reached.  The command window should display "ABORTING EXECUTE COMMAND".  The script should send another step with Dx = 1.  The Accept button should be blinking.</t>
+  </si>
+  <si>
+    <t>Press Accept and then Start.  While the ramp is running switch both Execute and Propose buttons to Auto.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type "testNtcpLink.pl --lbcb=? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--option=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the command window where ? Is the number of LBCBs you are controlling</t>
+    </r>
+  </si>
+  <si>
+    <t>The script will execute three steps.  At the fourth step the script will send a close-session command to the OM after the propose message.  At this point NTCP should disconnect and the Socket widget will disappear</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type "testNtcpLink.pl --lbcb=? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--option=2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the command window where ? Is the number of LBCBs you are controlling</t>
+    </r>
+  </si>
+  <si>
+    <t>The script will execute three steps.  At the fourth step the script will send a close-session command to the OM after the OM accepts the propose message.  At this point NTCP should disconnect and the Socket widget will disappear</t>
+  </si>
+  <si>
+    <t>The script will execute three steps.  At the fourth step the script will send a close-session command to the OM after the execute message.  At this point NTCP should disconnect and the Socket widget will disappear</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type "testNtcpLink.pl --lbcb=? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--option=3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the command window where ? Is the number of LBCBs you are controlling</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type "testNtcpLink.pl --lbcb=? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--option=4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the command window where ? Is the number of LBCBs you are controlling</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type "testNtcpLink.pl --lbcb=? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--option=5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the command window where ? Is the number of LBCBs you are controlling</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type "testNtcpLink.pl --lbcb=? </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--option=6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the command window where ? Is the number of LBCBs you are controlling</t>
+    </r>
+  </si>
+  <si>
+    <t>The script will execute three steps.  At the fourth step the script will send a close-session command to the OM after the OM finishes the ramp.  At this point NTCP should disconnect and the Socket widget will disappear</t>
+  </si>
+  <si>
+    <t>The script will execute three steps.  At the fourth step the script will send a close-session command to the OM after sending a get-control-point message.  At this point NTCP should disconnect and the Socket widget will disappear</t>
+  </si>
+  <si>
+    <t>The script will execute three steps.  At the fourth step the script will send a close-session command to the OM after the OM returns the control point data.  At this point NTCP should disconnect and the Socket widget will disappear</t>
+  </si>
+  <si>
+    <t>NTCP</t>
   </si>
 </sst>
 </file>
@@ -522,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -547,6 +835,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -558,15 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -909,170 +1200,170 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>100</v>
+      <c r="A9" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1092,10 +1383,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,457 +1416,463 @@
         <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>138</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
+      <c r="A6" s="15"/>
+      <c r="B6" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>145</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="6"/>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="6"/>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>149</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="6"/>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>151</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="6"/>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="6"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="6"/>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="6"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>8</v>
-      </c>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
       <c r="B15" s="4" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="4"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="6"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A17" s="15"/>
+      <c r="B17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="6"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A18" s="15"/>
+      <c r="B18" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="6"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A19" s="15"/>
+      <c r="B19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="6"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>9</v>
-      </c>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="6"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="15"/>
+      <c r="B21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="6"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>12</v>
-      </c>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="6"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>14</v>
-      </c>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
       <c r="B24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
       <c r="B25" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
       <c r="B26" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="6"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="6"/>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="6"/>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="6"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="6"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="6"/>
+      <c r="A32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>17</v>
-      </c>
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
       <c r="B34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>19</v>
-      </c>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="6"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="4"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="6"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>18</v>
-      </c>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="6"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>4</v>
-      </c>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="6"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>20</v>
-      </c>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="6"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A40" s="16"/>
+      <c r="B40" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="6"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="B41" s="4" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -1584,375 +1881,741 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
       <c r="B42" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
       <c r="B43" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
       <c r="B44" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>4</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="15"/>
       <c r="B45" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="15"/>
       <c r="B46" s="4" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
       <c r="B47" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
       <c r="B48" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
       <c r="B49" s="4" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
       <c r="B50" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="6"/>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
+      <c r="B51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C52" s="6"/>
+    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C53" s="6"/>
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="15"/>
+      <c r="B53" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="6"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="6"/>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="6"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>32</v>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>32</v>
+      <c r="A58" s="15"/>
+      <c r="B58" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A59" s="15"/>
+      <c r="B59" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" s="10"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="A60" s="15"/>
+      <c r="B60" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="10"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>35</v>
-      </c>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="15"/>
+      <c r="B61" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="10"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A62" s="15"/>
+      <c r="B62" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="10"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A63" s="15"/>
+      <c r="B63" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="10"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A64" s="15"/>
+      <c r="B64" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="10"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="A65" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="10"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
       <c r="B66" s="6" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
       <c r="B67" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="15"/>
       <c r="B68" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
+      <c r="B73" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="15"/>
+      <c r="B79" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="16"/>
+      <c r="B80" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="10"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="17"/>
+      <c r="B82" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="17"/>
+      <c r="B83" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="17"/>
+      <c r="B84" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" s="10"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="17"/>
+      <c r="B85" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="17"/>
+      <c r="B86" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="17"/>
+      <c r="B87" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="17"/>
+      <c r="B88" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="17"/>
+      <c r="B89" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="17"/>
+      <c r="B90" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="17"/>
+      <c r="B91" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="17"/>
+      <c r="B92" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="17"/>
+      <c r="B93" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A94" s="17"/>
+      <c r="B94" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="17"/>
+      <c r="B95" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="17"/>
+      <c r="B96" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="17"/>
+      <c r="B97" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="17"/>
+      <c r="B98" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A99" s="17"/>
+      <c r="B99" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="17"/>
+      <c r="B100" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A101" s="17"/>
+      <c r="B101" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="17"/>
+      <c r="B102" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A103" s="17"/>
+      <c r="B103" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A57:A72"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A33:A56"/>
+  <mergeCells count="7">
+    <mergeCell ref="A81:A103"/>
+    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="A11:A22"/>
+    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="A41:A64"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A65:A80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1963,15 +2626,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="11" customWidth="1"/>
     <col min="6" max="6" width="83.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1992,186 +2655,186 @@
         <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="16" t="s">
+      <c r="C10" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="16" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="16" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="16" t="s">
+      <c r="C13" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="16" t="s">
+      <c r="C14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="16" t="s">
+      <c r="C15" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Merge Combined Control with trunk r711:725
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
     <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
     <sheet name="Configuration Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Force Control Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="187">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -810,7 +811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -846,6 +847,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1200,7 +1204,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1213,7 +1217,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="6" t="s">
         <v>74</v>
       </c>
@@ -1224,7 +1228,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="6" t="s">
         <v>76</v>
       </c>
@@ -1235,7 +1239,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>79</v>
       </c>
@@ -1246,7 +1250,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
         <v>78</v>
       </c>
@@ -1257,7 +1261,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
         <v>81</v>
       </c>
@@ -1268,7 +1272,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="6" t="s">
         <v>84</v>
       </c>
@@ -1279,7 +1283,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>98</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1292,7 +1296,7 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="6" t="s">
         <v>78</v>
       </c>
@@ -1303,7 +1307,7 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
@@ -1314,7 +1318,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="6" t="s">
         <v>84</v>
       </c>
@@ -1325,7 +1329,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="6" t="s">
         <v>99</v>
       </c>
@@ -1336,7 +1340,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="6" t="s">
         <v>101</v>
       </c>
@@ -1347,7 +1351,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="6" t="s">
         <v>103</v>
       </c>
@@ -1358,7 +1362,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="6" t="s">
         <v>104</v>
       </c>
@@ -1385,8 +1389,8 @@
   </sheetPr>
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1438,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1448,7 +1452,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
         <v>138</v>
       </c>
@@ -1460,7 +1464,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>141</v>
       </c>
@@ -1472,7 +1476,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
         <v>139</v>
       </c>
@@ -1484,7 +1488,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
         <v>144</v>
       </c>
@@ -1496,7 +1500,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="10" t="s">
         <v>146</v>
       </c>
@@ -1508,7 +1512,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="10" t="s">
         <v>148</v>
       </c>
@@ -1520,7 +1524,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="10" t="s">
         <v>150</v>
       </c>
@@ -1532,7 +1536,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1546,7 +1550,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1556,7 +1560,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1568,7 +1572,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1580,7 +1584,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -1592,7 +1596,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
@@ -1602,7 +1606,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="6" t="s">
         <v>88</v>
       </c>
@@ -1612,7 +1616,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="6" t="s">
         <v>89</v>
       </c>
@@ -1622,7 +1626,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
@@ -1632,7 +1636,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="6" t="s">
         <v>91</v>
       </c>
@@ -1642,7 +1646,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="6" t="s">
         <v>92</v>
       </c>
@@ -1652,7 +1656,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="6" t="s">
         <v>110</v>
       </c>
@@ -1662,7 +1666,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1676,7 +1680,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1686,7 +1690,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="4" t="s">
         <v>41</v>
       </c>
@@ -1698,7 +1702,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
@@ -1710,7 +1714,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1722,7 +1726,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1734,7 +1738,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
@@ -1746,7 +1750,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
@@ -1758,7 +1762,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1770,7 +1774,7 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1784,7 +1788,7 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="4" t="s">
         <v>46</v>
       </c>
@@ -1796,7 +1800,7 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
@@ -1808,7 +1812,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="6" t="s">
         <v>87</v>
       </c>
@@ -1818,7 +1822,7 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
@@ -1828,7 +1832,7 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="6" t="s">
         <v>89</v>
       </c>
@@ -1838,7 +1842,7 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="6" t="s">
         <v>90</v>
       </c>
@@ -1848,7 +1852,7 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="6" t="s">
         <v>91</v>
       </c>
@@ -1858,7 +1862,7 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="17"/>
       <c r="B40" s="6" t="s">
         <v>94</v>
       </c>
@@ -1868,7 +1872,7 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1882,7 +1886,7 @@
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="4" t="s">
         <v>40</v>
       </c>
@@ -1892,7 +1896,7 @@
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1904,7 +1908,7 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="4" t="s">
         <v>48</v>
       </c>
@@ -1914,7 +1918,7 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="4" t="s">
         <v>49</v>
       </c>
@@ -1926,7 +1930,7 @@
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="4" t="s">
         <v>68</v>
       </c>
@@ -1938,7 +1942,7 @@
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="4" t="s">
         <v>50</v>
       </c>
@@ -1950,7 +1954,7 @@
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="4" t="s">
         <v>51</v>
       </c>
@@ -1962,7 +1966,7 @@
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="4" t="s">
         <v>69</v>
       </c>
@@ -1974,7 +1978,7 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
@@ -1986,7 +1990,7 @@
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="4" t="s">
         <v>52</v>
       </c>
@@ -1998,7 +2002,7 @@
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="4" t="s">
         <v>70</v>
       </c>
@@ -2010,7 +2014,7 @@
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="4" t="s">
         <v>44</v>
       </c>
@@ -2022,7 +2026,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="4" t="s">
         <v>51</v>
       </c>
@@ -2034,7 +2038,7 @@
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="4" t="s">
         <v>53</v>
       </c>
@@ -2046,7 +2050,7 @@
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="4" t="s">
         <v>54</v>
       </c>
@@ -2058,7 +2062,7 @@
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="10" t="s">
         <v>44</v>
       </c>
@@ -2070,7 +2074,7 @@
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="10" t="s">
         <v>55</v>
       </c>
@@ -2082,7 +2086,7 @@
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="10" t="s">
         <v>87</v>
       </c>
@@ -2092,7 +2096,7 @@
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="10" t="s">
         <v>88</v>
       </c>
@@ -2102,7 +2106,7 @@
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="10" t="s">
         <v>89</v>
       </c>
@@ -2112,7 +2116,7 @@
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="10" t="s">
         <v>90</v>
       </c>
@@ -2122,7 +2126,7 @@
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
+      <c r="A63" s="16"/>
       <c r="B63" s="10" t="s">
         <v>91</v>
       </c>
@@ -2132,7 +2136,7 @@
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+      <c r="A64" s="16"/>
       <c r="B64" s="10" t="s">
         <v>92</v>
       </c>
@@ -2142,7 +2146,7 @@
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B65" s="10" t="s">
@@ -2154,7 +2158,7 @@
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="6" t="s">
         <v>152</v>
       </c>
@@ -2166,7 +2170,7 @@
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="6" t="s">
         <v>56</v>
       </c>
@@ -2178,7 +2182,7 @@
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="6" t="s">
         <v>57</v>
       </c>
@@ -2190,7 +2194,7 @@
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="6" t="s">
         <v>41</v>
       </c>
@@ -2202,7 +2206,7 @@
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="6" t="s">
         <v>58</v>
       </c>
@@ -2214,7 +2218,7 @@
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
+      <c r="A71" s="16"/>
       <c r="B71" s="6" t="s">
         <v>56</v>
       </c>
@@ -2226,7 +2230,7 @@
       <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="6" t="s">
         <v>57</v>
       </c>
@@ -2238,7 +2242,7 @@
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="6" t="s">
         <v>59</v>
       </c>
@@ -2250,7 +2254,7 @@
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
+      <c r="A74" s="16"/>
       <c r="B74" s="6" t="s">
         <v>60</v>
       </c>
@@ -2262,7 +2266,7 @@
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
+      <c r="A75" s="16"/>
       <c r="B75" s="6" t="s">
         <v>61</v>
       </c>
@@ -2274,7 +2278,7 @@
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
+      <c r="A76" s="16"/>
       <c r="B76" s="6" t="s">
         <v>62</v>
       </c>
@@ -2286,7 +2290,7 @@
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
+      <c r="A77" s="16"/>
       <c r="B77" s="6" t="s">
         <v>56</v>
       </c>
@@ -2298,7 +2302,7 @@
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
+      <c r="A78" s="16"/>
       <c r="B78" s="6" t="s">
         <v>64</v>
       </c>
@@ -2310,7 +2314,7 @@
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
+      <c r="A79" s="16"/>
       <c r="B79" s="6" t="s">
         <v>66</v>
       </c>
@@ -2322,7 +2326,7 @@
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="6" t="s">
         <v>56</v>
       </c>
@@ -2334,7 +2338,7 @@
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="18" t="s">
         <v>186</v>
       </c>
       <c r="B81" s="10" t="s">
@@ -2346,7 +2350,7 @@
       <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
+      <c r="A82" s="18"/>
       <c r="B82" s="10" t="s">
         <v>155</v>
       </c>
@@ -2358,7 +2362,7 @@
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="10" t="s">
         <v>157</v>
       </c>
@@ -2370,7 +2374,7 @@
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
+      <c r="A84" s="18"/>
       <c r="B84" s="10" t="s">
         <v>159</v>
       </c>
@@ -2380,7 +2384,7 @@
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
+      <c r="A85" s="18"/>
       <c r="B85" s="10" t="s">
         <v>160</v>
       </c>
@@ -2392,7 +2396,7 @@
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
+      <c r="A86" s="18"/>
       <c r="B86" s="10" t="s">
         <v>162</v>
       </c>
@@ -2404,7 +2408,7 @@
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
+      <c r="A87" s="18"/>
       <c r="B87" s="10" t="s">
         <v>50</v>
       </c>
@@ -2416,7 +2420,7 @@
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
+      <c r="A88" s="18"/>
       <c r="B88" s="10" t="s">
         <v>165</v>
       </c>
@@ -2428,7 +2432,7 @@
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
+      <c r="A89" s="18"/>
       <c r="B89" s="10" t="s">
         <v>167</v>
       </c>
@@ -2440,7 +2444,7 @@
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
+      <c r="A90" s="18"/>
       <c r="B90" s="10" t="s">
         <v>171</v>
       </c>
@@ -2452,7 +2456,7 @@
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
+      <c r="A91" s="18"/>
       <c r="B91" s="10" t="s">
         <v>169</v>
       </c>
@@ -2464,7 +2468,7 @@
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
+      <c r="A92" s="18"/>
       <c r="B92" s="10" t="s">
         <v>174</v>
       </c>
@@ -2476,7 +2480,7 @@
       <c r="F92" s="5"/>
     </row>
     <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
+      <c r="A93" s="18"/>
       <c r="B93" s="10" t="s">
         <v>173</v>
       </c>
@@ -2488,7 +2492,7 @@
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
+      <c r="A94" s="18"/>
       <c r="B94" s="10" t="s">
         <v>176</v>
       </c>
@@ -2500,7 +2504,7 @@
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
+      <c r="A95" s="18"/>
       <c r="B95" s="10" t="s">
         <v>173</v>
       </c>
@@ -2512,7 +2516,7 @@
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
+      <c r="A96" s="18"/>
       <c r="B96" s="10" t="s">
         <v>179</v>
       </c>
@@ -2524,7 +2528,7 @@
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
+      <c r="A97" s="18"/>
       <c r="B97" s="10" t="s">
         <v>173</v>
       </c>
@@ -2536,7 +2540,7 @@
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
+      <c r="A98" s="18"/>
       <c r="B98" s="10" t="s">
         <v>180</v>
       </c>
@@ -2548,7 +2552,7 @@
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
+      <c r="A99" s="18"/>
       <c r="B99" s="10" t="s">
         <v>173</v>
       </c>
@@ -2560,7 +2564,7 @@
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
+      <c r="A100" s="18"/>
       <c r="B100" s="10" t="s">
         <v>181</v>
       </c>
@@ -2572,7 +2576,7 @@
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
+      <c r="A101" s="18"/>
       <c r="B101" s="10" t="s">
         <v>173</v>
       </c>
@@ -2584,7 +2588,7 @@
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
+      <c r="A102" s="18"/>
       <c r="B102" s="10" t="s">
         <v>182</v>
       </c>
@@ -2596,7 +2600,7 @@
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
+      <c r="A103" s="18"/>
       <c r="B103" s="10" t="s">
         <v>173</v>
       </c>
@@ -2609,13 +2613,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A65:A80"/>
     <mergeCell ref="A81:A103"/>
     <mergeCell ref="A23:A31"/>
     <mergeCell ref="A11:A22"/>
     <mergeCell ref="A32:A40"/>
     <mergeCell ref="A41:A64"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A65:A80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2659,7 +2663,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2671,7 +2675,7 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="7" t="s">
         <v>112</v>
       </c>
@@ -2683,7 +2687,7 @@
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="13" t="s">
         <v>116</v>
       </c>
@@ -2695,7 +2699,7 @@
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="13" t="s">
         <v>118</v>
       </c>
@@ -2707,7 +2711,7 @@
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="13" t="s">
         <v>119</v>
       </c>
@@ -2717,7 +2721,7 @@
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="13" t="s">
         <v>120</v>
       </c>
@@ -2729,7 +2733,7 @@
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="13" t="s">
         <v>122</v>
       </c>
@@ -2741,7 +2745,7 @@
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="13" t="s">
         <v>125</v>
       </c>
@@ -2753,7 +2757,7 @@
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="13" t="s">
         <v>126</v>
       </c>
@@ -2765,7 +2769,7 @@
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="13" t="s">
         <v>129</v>
       </c>
@@ -2777,7 +2781,7 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="13" t="s">
         <v>130</v>
       </c>
@@ -2789,7 +2793,7 @@
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="13" t="s">
         <v>131</v>
       </c>
@@ -2801,7 +2805,7 @@
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="13" t="s">
         <v>132</v>
       </c>
@@ -2813,7 +2817,7 @@
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="13" t="s">
         <v>133</v>
       </c>
@@ -2825,7 +2829,7 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="13" t="s">
         <v>134</v>
       </c>
@@ -2843,4 +2847,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Menu entries and configuration tests
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
     <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
     <sheet name="Configuration Tests" sheetId="3" r:id="rId3"/>
-    <sheet name="Force Control Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="205">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -716,6 +715,60 @@
   </si>
   <si>
     <t>NTCP</t>
+  </si>
+  <si>
+    <t>Operation Manager Configuration Test</t>
+  </si>
+  <si>
+    <t>Select the Edit-&gt;Position menu item</t>
+  </si>
+  <si>
+    <t>The LBCB Position widget should appear</t>
+  </si>
+  <si>
+    <t>Change all of the position  values to unique values  and press OK.  Do this for both LBCBs</t>
+  </si>
+  <si>
+    <t>Reselect Edit-&gt;Position</t>
+  </si>
+  <si>
+    <t>Verify that all of the values are still changed</t>
+  </si>
+  <si>
+    <t>Press OK</t>
+  </si>
+  <si>
+    <t>Restart the LBCB Operation Manager program.  Select Edit-&gt;Position again</t>
+  </si>
+  <si>
+    <t>Verify that all of the values have returned to their original values.</t>
+  </si>
+  <si>
+    <t>Select File-&gt;Save and restart the program</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Position again</t>
+  </si>
+  <si>
+    <t>Verify that the values change when they are supposed to.</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Middle Loop</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Mixed Mode Loop</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Timing &amp; Logging</t>
+  </si>
+  <si>
+    <t>Repeat the test for the "Auto Balance Control" and "Auto Balance Error Window" in the Autobalance tab</t>
+  </si>
+  <si>
+    <t>Repeat the test for the stiffness matrix, Jacobian Gain, Max Increment, Force Group Priorities, Force Error Range, Stiffness Limits, and Force Control Parameters  in the Mixed Mode tab</t>
+  </si>
+  <si>
+    <t>Repeat this test with Edit-&gt;Limits.  Note There are 16 different displays when selecting a limit set and an LBCB</t>
   </si>
 </sst>
 </file>
@@ -848,7 +901,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1175,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,7 +1443,7 @@
   <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2840,66 +2893,186 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Force Control Test
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
     <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
     <sheet name="Configuration Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Force Control Tests" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="225">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -769,6 +770,66 @@
   </si>
   <si>
     <t>Repeat this test with Edit-&gt;Limits.  Note There are 16 different displays when selecting a limit set and an LBCB</t>
+  </si>
+  <si>
+    <t>This test needs a rubber specimen connected.  Real Startup procedure needs to done first.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the cartesian force limits to a window that is within the capacity of the rubber specimen.  Move the LBCB a small amount in to translation and two rotation directions.  The translation should be &gt; 0.1 inches.  The rotation should be &gt; .001 radians.  Make sure that none of the translations add tension to the specimen.  </t>
+  </si>
+  <si>
+    <t>Enter ramp times of 2 seconds for all of the ramp entries in the Mixed Mode Window.    Switch the LBCB Operation Manager Window to Mixed Mode.  Set the Jacobian to 0.8 for all DOFs.  Set the max increment to .01 for all translations and .0001 for all rotations.  Set all Force Group Priorities to 5.  Set the Force Error Range to 5 lbs for for the forces and 20 lbs*inches for the moments.  Set the low stiffness limit to 20 and the high limit to 1E+6.  Make sure that all of the force control parameters are set to "No".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the LBCB Operation Manager Window you will see the Convergence display indicating which DOFs are converged as well as which DOF is being controlled.  The stiffness matrix will have updated values for the column associated with the controlling DOF.  The Target display will show for the controlling DOF a displacement that equals the current displacement plus the max increment.  The last step will be slightly less than the max increment.  The force ramp should end with all of the force DOFs converged.  The resulting forces and moments should be 0 +/- the force error </t>
+  </si>
+  <si>
+    <t>The changed DOF will converge to the tighter force error range.</t>
+  </si>
+  <si>
+    <t>You should see a significant increase in force along the directions that are displaced.  Record these force values as force target 1.</t>
+  </si>
+  <si>
+    <t>Make sure that the force DOF with the changed Max Increment shows a displacement in the LBCB Operation Manager Target window that is the current displacement +/- .03.</t>
+  </si>
+  <si>
+    <t>In the Mixed Mode Window set the forces moments which are in the same directions as the displacement DOFs  set earlier to zero.   Press Set Target then Start on the Mixed Mode Window.</t>
+  </si>
+  <si>
+    <t>Enter the forces for target 1 in the Mixed Mode Widget.  Press Set Target and Start</t>
+  </si>
+  <si>
+    <t>The force ramp should stop on a limit fault for the limit that was changed</t>
+  </si>
+  <si>
+    <t>Take a look at which controlling DOF is chosen.  In the previous ramps the moments were chosen first.  In this case the force DOF with the 3 lb force error range should be chosen first.</t>
+  </si>
+  <si>
+    <t>The controlling DOF that is chosen should follow the priorities with the lowest adjusted first.</t>
+  </si>
+  <si>
+    <t>The stiffness matrix will not be updated during this camp.  The controlling DOFs will first adjust all of the DOFs with the lower priority and then it will adjust all of the DOFs in the in the higher party.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the force error range for one of the force DOFs to 3 lbs.  Press Set Target and Start again.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set a limit for one of the target 1 forces to be just under the target 1 magnitude.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, reset the Max Increment to .01 inches.  Set the Force Control Parameter "Use Force Error Range Ratios" to Yes.  Enter the forces for target 1 and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Use Force Error Range Ratios" to No.  Set the Force Control Paraemter "Use Group Priorities" to Yes.  Enter a different priority for each DOF in the Force Group Priorities display between 0 and 5.  Enter zero for the forces and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Multi Command Update" to Yes.  Enter two  different priorities for the DOF in the Force Group Priorities display.  Enter the target 1 forces and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>Force Control Test</t>
+  </si>
+  <si>
+    <t>After the ramp is stopped, set the Max increment for one of the force DOFs to .03 inches.  Enter zero for all of the forces in the Mixed Mode Widget.  Press Set Target and Start</t>
   </si>
 </sst>
 </file>
@@ -864,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -907,6 +968,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -925,6 +995,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,7 +1335,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1270,7 +1348,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="6" t="s">
         <v>74</v>
       </c>
@@ -1281,7 +1359,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="6" t="s">
         <v>76</v>
       </c>
@@ -1292,7 +1370,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="6" t="s">
         <v>79</v>
       </c>
@@ -1303,7 +1381,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="6" t="s">
         <v>78</v>
       </c>
@@ -1314,7 +1392,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="6" t="s">
         <v>81</v>
       </c>
@@ -1325,7 +1403,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="6" t="s">
         <v>84</v>
       </c>
@@ -1336,7 +1414,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="18" t="s">
         <v>98</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1349,7 +1427,7 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
         <v>78</v>
       </c>
@@ -1360,7 +1438,7 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
@@ -1371,7 +1449,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="6" t="s">
         <v>84</v>
       </c>
@@ -1382,7 +1460,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="6" t="s">
         <v>99</v>
       </c>
@@ -1393,7 +1471,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="6" t="s">
         <v>101</v>
       </c>
@@ -1404,7 +1482,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="6" t="s">
         <v>103</v>
       </c>
@@ -1415,7 +1493,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="6" t="s">
         <v>104</v>
       </c>
@@ -1443,7 +1521,7 @@
   <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,7 +1569,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1505,7 +1583,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="4" t="s">
         <v>138</v>
       </c>
@@ -1517,7 +1595,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="6" t="s">
         <v>141</v>
       </c>
@@ -1529,7 +1607,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="6" t="s">
         <v>139</v>
       </c>
@@ -1541,7 +1619,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="6" t="s">
         <v>144</v>
       </c>
@@ -1553,7 +1631,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="10" t="s">
         <v>146</v>
       </c>
@@ -1565,7 +1643,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
         <v>148</v>
       </c>
@@ -1577,7 +1655,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="10" t="s">
         <v>150</v>
       </c>
@@ -1589,7 +1667,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1603,7 +1681,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1613,7 +1691,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1625,7 +1703,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1637,7 +1715,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -1649,7 +1727,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
@@ -1659,7 +1737,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="6" t="s">
         <v>88</v>
       </c>
@@ -1669,7 +1747,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="6" t="s">
         <v>89</v>
       </c>
@@ -1679,7 +1757,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
@@ -1689,7 +1767,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="6" t="s">
         <v>91</v>
       </c>
@@ -1699,7 +1777,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="6" t="s">
         <v>92</v>
       </c>
@@ -1709,7 +1787,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="6" t="s">
         <v>110</v>
       </c>
@@ -1719,7 +1797,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1733,7 +1811,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1743,7 +1821,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="4" t="s">
         <v>41</v>
       </c>
@@ -1755,7 +1833,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
@@ -1767,7 +1845,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1779,7 +1857,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1791,7 +1869,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
@@ -1803,7 +1881,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
@@ -1815,7 +1893,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1827,7 +1905,7 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1841,7 +1919,7 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="4" t="s">
         <v>46</v>
       </c>
@@ -1853,7 +1931,7 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
@@ -1865,7 +1943,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="6" t="s">
         <v>87</v>
       </c>
@@ -1875,7 +1953,7 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
@@ -1885,7 +1963,7 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="6" t="s">
         <v>89</v>
       </c>
@@ -1895,7 +1973,7 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="6" t="s">
         <v>90</v>
       </c>
@@ -1905,7 +1983,7 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="6" t="s">
         <v>91</v>
       </c>
@@ -1915,7 +1993,7 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+      <c r="A40" s="20"/>
       <c r="B40" s="6" t="s">
         <v>94</v>
       </c>
@@ -1925,7 +2003,7 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1939,7 +2017,7 @@
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="4" t="s">
         <v>40</v>
       </c>
@@ -1949,7 +2027,7 @@
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1961,7 +2039,7 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="4" t="s">
         <v>48</v>
       </c>
@@ -1971,7 +2049,7 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="4" t="s">
         <v>49</v>
       </c>
@@ -1983,7 +2061,7 @@
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="4" t="s">
         <v>68</v>
       </c>
@@ -1995,7 +2073,7 @@
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="4" t="s">
         <v>50</v>
       </c>
@@ -2007,7 +2085,7 @@
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="4" t="s">
         <v>51</v>
       </c>
@@ -2019,7 +2097,7 @@
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="4" t="s">
         <v>69</v>
       </c>
@@ -2031,7 +2109,7 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="4" t="s">
         <v>46</v>
       </c>
@@ -2043,7 +2121,7 @@
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="4" t="s">
         <v>52</v>
       </c>
@@ -2055,7 +2133,7 @@
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="4" t="s">
         <v>70</v>
       </c>
@@ -2067,7 +2145,7 @@
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="4" t="s">
         <v>44</v>
       </c>
@@ -2079,7 +2157,7 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="4" t="s">
         <v>51</v>
       </c>
@@ -2091,7 +2169,7 @@
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="4" t="s">
         <v>53</v>
       </c>
@@ -2103,7 +2181,7 @@
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="4" t="s">
         <v>54</v>
       </c>
@@ -2115,7 +2193,7 @@
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="10" t="s">
         <v>44</v>
       </c>
@@ -2127,7 +2205,7 @@
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="10" t="s">
         <v>55</v>
       </c>
@@ -2139,7 +2217,7 @@
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="10" t="s">
         <v>87</v>
       </c>
@@ -2149,7 +2227,7 @@
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="10" t="s">
         <v>88</v>
       </c>
@@ -2159,7 +2237,7 @@
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="10" t="s">
         <v>89</v>
       </c>
@@ -2169,7 +2247,7 @@
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="10" t="s">
         <v>90</v>
       </c>
@@ -2179,7 +2257,7 @@
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="10" t="s">
         <v>91</v>
       </c>
@@ -2189,7 +2267,7 @@
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="10" t="s">
         <v>92</v>
       </c>
@@ -2199,7 +2277,7 @@
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="19" t="s">
         <v>31</v>
       </c>
       <c r="B65" s="10" t="s">
@@ -2211,7 +2289,7 @@
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="6" t="s">
         <v>152</v>
       </c>
@@ -2223,7 +2301,7 @@
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="6" t="s">
         <v>56</v>
       </c>
@@ -2235,7 +2313,7 @@
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="6" t="s">
         <v>57</v>
       </c>
@@ -2247,7 +2325,7 @@
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="6" t="s">
         <v>41</v>
       </c>
@@ -2259,7 +2337,7 @@
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="6" t="s">
         <v>58</v>
       </c>
@@ -2271,7 +2349,7 @@
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="6" t="s">
         <v>56</v>
       </c>
@@ -2283,7 +2361,7 @@
       <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="6" t="s">
         <v>57</v>
       </c>
@@ -2295,7 +2373,7 @@
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="6" t="s">
         <v>59</v>
       </c>
@@ -2307,7 +2385,7 @@
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="6" t="s">
         <v>60</v>
       </c>
@@ -2319,7 +2397,7 @@
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="6" t="s">
         <v>61</v>
       </c>
@@ -2331,7 +2409,7 @@
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="16"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="6" t="s">
         <v>62</v>
       </c>
@@ -2343,7 +2421,7 @@
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="6" t="s">
         <v>56</v>
       </c>
@@ -2355,7 +2433,7 @@
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="16"/>
+      <c r="A78" s="19"/>
       <c r="B78" s="6" t="s">
         <v>64</v>
       </c>
@@ -2367,7 +2445,7 @@
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
+      <c r="A79" s="19"/>
       <c r="B79" s="6" t="s">
         <v>66</v>
       </c>
@@ -2379,7 +2457,7 @@
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
+      <c r="A80" s="20"/>
       <c r="B80" s="6" t="s">
         <v>56</v>
       </c>
@@ -2391,7 +2469,7 @@
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="21" t="s">
         <v>186</v>
       </c>
       <c r="B81" s="10" t="s">
@@ -2403,7 +2481,7 @@
       <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="10" t="s">
         <v>155</v>
       </c>
@@ -2415,7 +2493,7 @@
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
+      <c r="A83" s="21"/>
       <c r="B83" s="10" t="s">
         <v>157</v>
       </c>
@@ -2427,7 +2505,7 @@
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
+      <c r="A84" s="21"/>
       <c r="B84" s="10" t="s">
         <v>159</v>
       </c>
@@ -2437,7 +2515,7 @@
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
+      <c r="A85" s="21"/>
       <c r="B85" s="10" t="s">
         <v>160</v>
       </c>
@@ -2449,7 +2527,7 @@
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
+      <c r="A86" s="21"/>
       <c r="B86" s="10" t="s">
         <v>162</v>
       </c>
@@ -2461,7 +2539,7 @@
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
+      <c r="A87" s="21"/>
       <c r="B87" s="10" t="s">
         <v>50</v>
       </c>
@@ -2473,7 +2551,7 @@
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="10" t="s">
         <v>165</v>
       </c>
@@ -2485,7 +2563,7 @@
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="18"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="10" t="s">
         <v>167</v>
       </c>
@@ -2497,7 +2575,7 @@
       <c r="F89" s="5"/>
     </row>
     <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="18"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="10" t="s">
         <v>171</v>
       </c>
@@ -2509,7 +2587,7 @@
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="18"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="10" t="s">
         <v>169</v>
       </c>
@@ -2521,7 +2599,7 @@
       <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="18"/>
+      <c r="A92" s="21"/>
       <c r="B92" s="10" t="s">
         <v>174</v>
       </c>
@@ -2533,7 +2611,7 @@
       <c r="F92" s="5"/>
     </row>
     <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="18"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="10" t="s">
         <v>173</v>
       </c>
@@ -2545,7 +2623,7 @@
       <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="10" t="s">
         <v>176</v>
       </c>
@@ -2557,7 +2635,7 @@
       <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="10" t="s">
         <v>173</v>
       </c>
@@ -2569,7 +2647,7 @@
       <c r="F95" s="5"/>
     </row>
     <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="18"/>
+      <c r="A96" s="21"/>
       <c r="B96" s="10" t="s">
         <v>179</v>
       </c>
@@ -2581,7 +2659,7 @@
       <c r="F96" s="5"/>
     </row>
     <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="10" t="s">
         <v>173</v>
       </c>
@@ -2593,7 +2671,7 @@
       <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="18"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="10" t="s">
         <v>180</v>
       </c>
@@ -2605,7 +2683,7 @@
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="18"/>
+      <c r="A99" s="21"/>
       <c r="B99" s="10" t="s">
         <v>173</v>
       </c>
@@ -2617,7 +2695,7 @@
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="10" t="s">
         <v>181</v>
       </c>
@@ -2629,7 +2707,7 @@
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="18"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="10" t="s">
         <v>173</v>
       </c>
@@ -2641,7 +2719,7 @@
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="18"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="10" t="s">
         <v>182</v>
       </c>
@@ -2653,7 +2731,7 @@
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="18"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="10" t="s">
         <v>173</v>
       </c>
@@ -2683,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2716,7 +2794,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2728,7 +2806,7 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="7" t="s">
         <v>112</v>
       </c>
@@ -2740,7 +2818,7 @@
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="13" t="s">
         <v>116</v>
       </c>
@@ -2752,7 +2830,7 @@
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="13" t="s">
         <v>118</v>
       </c>
@@ -2764,7 +2842,7 @@
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="13" t="s">
         <v>119</v>
       </c>
@@ -2774,7 +2852,7 @@
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="13" t="s">
         <v>120</v>
       </c>
@@ -2786,7 +2864,7 @@
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="13" t="s">
         <v>122</v>
       </c>
@@ -2798,7 +2876,7 @@
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="13" t="s">
         <v>125</v>
       </c>
@@ -2810,7 +2888,7 @@
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="13" t="s">
         <v>126</v>
       </c>
@@ -2822,7 +2900,7 @@
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="13" t="s">
         <v>129</v>
       </c>
@@ -2834,7 +2912,7 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="13" t="s">
         <v>130</v>
       </c>
@@ -2846,7 +2924,7 @@
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="13" t="s">
         <v>131</v>
       </c>
@@ -2858,7 +2936,7 @@
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="13" t="s">
         <v>132</v>
       </c>
@@ -2870,7 +2948,7 @@
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="13" t="s">
         <v>133</v>
       </c>
@@ -2882,7 +2960,7 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="13" t="s">
         <v>134</v>
       </c>
@@ -2894,7 +2972,7 @@
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="21" t="s">
         <v>187</v>
       </c>
       <c r="B17" s="14" t="s">
@@ -2908,7 +2986,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="13" t="s">
         <v>188</v>
       </c>
@@ -2920,7 +2998,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="13" t="s">
         <v>190</v>
       </c>
@@ -2930,7 +3008,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="13" t="s">
         <v>191</v>
       </c>
@@ -2942,7 +3020,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="13" t="s">
         <v>193</v>
       </c>
@@ -2952,7 +3030,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="13" t="s">
         <v>194</v>
       </c>
@@ -2964,7 +3042,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="13" t="s">
         <v>190</v>
       </c>
@@ -2974,7 +3052,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="13" t="s">
         <v>196</v>
       </c>
@@ -2984,7 +3062,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="13" t="s">
         <v>197</v>
       </c>
@@ -2996,7 +3074,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="13" t="s">
         <v>204</v>
       </c>
@@ -3008,7 +3086,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="13" t="s">
         <v>199</v>
       </c>
@@ -3020,7 +3098,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="13" t="s">
         <v>200</v>
       </c>
@@ -3032,7 +3110,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="13" t="s">
         <v>201</v>
       </c>
@@ -3044,7 +3122,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="13" t="s">
         <v>202</v>
       </c>
@@ -3056,7 +3134,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="13" t="s">
         <v>203</v>
       </c>
@@ -3075,4 +3153,204 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+    </row>
+    <row r="15" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Branch from CombinedControl 809 for Wharf Pier Test
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19320" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
-    <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
-    <sheet name="Configuration Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="OM Setup Test" sheetId="3" r:id="rId2"/>
+    <sheet name="No Oil Test" sheetId="1" r:id="rId3"/>
+    <sheet name="Oil Test with Free LBCB(s)" sheetId="6" r:id="rId4"/>
+    <sheet name="Rubber Specimen Test" sheetId="4" r:id="rId5"/>
+    <sheet name="Fake Startup" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="231">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -715,6 +718,138 @@
   </si>
   <si>
     <t>NTCP</t>
+  </si>
+  <si>
+    <t>Operation Manager Configuration Test</t>
+  </si>
+  <si>
+    <t>Select the Edit-&gt;Position menu item</t>
+  </si>
+  <si>
+    <t>The LBCB Position widget should appear</t>
+  </si>
+  <si>
+    <t>Change all of the position  values to unique values  and press OK.  Do this for both LBCBs</t>
+  </si>
+  <si>
+    <t>Reselect Edit-&gt;Position</t>
+  </si>
+  <si>
+    <t>Verify that all of the values are still changed</t>
+  </si>
+  <si>
+    <t>Press OK</t>
+  </si>
+  <si>
+    <t>Restart the LBCB Operation Manager program.  Select Edit-&gt;Position again</t>
+  </si>
+  <si>
+    <t>Verify that all of the values have returned to their original values.</t>
+  </si>
+  <si>
+    <t>Select File-&gt;Save and restart the program</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Position again</t>
+  </si>
+  <si>
+    <t>Verify that the values change when they are supposed to.</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Middle Loop</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Mixed Mode Loop</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Timing &amp; Logging</t>
+  </si>
+  <si>
+    <t>Repeat the test for the "Auto Balance Control" and "Auto Balance Error Window" in the Autobalance tab</t>
+  </si>
+  <si>
+    <t>Repeat the test for the stiffness matrix, Jacobian Gain, Max Increment, Force Group Priorities, Force Error Range, Stiffness Limits, and Force Control Parameters  in the Mixed Mode tab</t>
+  </si>
+  <si>
+    <t>Repeat this test with Edit-&gt;Limits.  Note There are 16 different displays when selecting a limit set and an LBCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the cartesian force limits to a window that is within the capacity of the rubber specimen.  Move the LBCB a small amount in to translation and two rotation directions.  The translation should be &gt; 0.1 inches.  The rotation should be &gt; .001 radians.  Make sure that none of the translations add tension to the specimen.  </t>
+  </si>
+  <si>
+    <t>Enter ramp times of 2 seconds for all of the ramp entries in the Mixed Mode Window.    Switch the LBCB Operation Manager Window to Mixed Mode.  Set the Jacobian to 0.8 for all DOFs.  Set the max increment to .01 for all translations and .0001 for all rotations.  Set all Force Group Priorities to 5.  Set the Force Error Range to 5 lbs for for the forces and 20 lbs*inches for the moments.  Set the low stiffness limit to 20 and the high limit to 1E+6.  Make sure that all of the force control parameters are set to "No".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the LBCB Operation Manager Window you will see the Convergence display indicating which DOFs are converged as well as which DOF is being controlled.  The stiffness matrix will have updated values for the column associated with the controlling DOF.  The Target display will show for the controlling DOF a displacement that equals the current displacement plus the max increment.  The last step will be slightly less than the max increment.  The force ramp should end with all of the force DOFs converged.  The resulting forces and moments should be 0 +/- the force error </t>
+  </si>
+  <si>
+    <t>The changed DOF will converge to the tighter force error range.</t>
+  </si>
+  <si>
+    <t>You should see a significant increase in force along the directions that are displaced.  Record these force values as force target 1.</t>
+  </si>
+  <si>
+    <t>Make sure that the force DOF with the changed Max Increment shows a displacement in the LBCB Operation Manager Target window that is the current displacement +/- .03.</t>
+  </si>
+  <si>
+    <t>In the Mixed Mode Window set the forces moments which are in the same directions as the displacement DOFs  set earlier to zero.   Press Set Target then Start on the Mixed Mode Window.</t>
+  </si>
+  <si>
+    <t>Enter the forces for target 1 in the Mixed Mode Widget.  Press Set Target and Start</t>
+  </si>
+  <si>
+    <t>The force ramp should stop on a limit fault for the limit that was changed</t>
+  </si>
+  <si>
+    <t>Take a look at which controlling DOF is chosen.  In the previous ramps the moments were chosen first.  In this case the force DOF with the 3 lb force error range should be chosen first.</t>
+  </si>
+  <si>
+    <t>The controlling DOF that is chosen should follow the priorities with the lowest adjusted first.</t>
+  </si>
+  <si>
+    <t>The stiffness matrix will not be updated during this camp.  The controlling DOFs will first adjust all of the DOFs with the lower priority and then it will adjust all of the DOFs in the in the higher party.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the force error range for one of the force DOFs to 3 lbs.  Press Set Target and Start again.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set a limit for one of the target 1 forces to be just under the target 1 magnitude.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, reset the Max Increment to .01 inches.  Set the Force Control Parameter "Use Force Error Range Ratios" to Yes.  Enter the forces for target 1 and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Use Force Error Range Ratios" to No.  Set the Force Control Paraemter "Use Group Priorities" to Yes.  Enter a different priority for each DOF in the Force Group Priorities display between 0 and 5.  Enter zero for the forces and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Multi Command Update" to Yes.  Enter two  different priorities for the DOF in the Force Group Priorities display.  Enter the target 1 forces and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>Force Control Test</t>
+  </si>
+  <si>
+    <t>After the ramp is stopped, set the Max increment for one of the force DOFs to .03 inches.  Enter zero for all of the forces in the Mixed Mode Widget.  Press Set Target and Start</t>
+  </si>
+  <si>
+    <t>Turn On Oil</t>
+  </si>
+  <si>
+    <t>This test needs a rigid rubber specimen connected.  The Startup procedure including oil turn on needs to done first.</t>
+  </si>
+  <si>
+    <t>The LBCB(s) should move for 10 seconds to the commanded displacement. The measured displacement should be the same as the commanded displacement when the offset is taken into account.</t>
+  </si>
+  <si>
+    <t>Input a target of displacement Dx within the displacement limits and press "Set Target".  Record the difference between the command displacement and the measured displacment as an offset.</t>
+  </si>
+  <si>
+    <t>Set Rigid Connection to "Yes".  Save the change.</t>
+  </si>
+  <si>
+    <t>Verify that the Rigid Connection is still "Yes".</t>
+  </si>
+  <si>
+    <t>Verify that LBCB2 cannot be selected for the Mixed Mode, and Cartesian Limits pages.</t>
   </si>
 </sst>
 </file>
@@ -810,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -847,6 +982,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -854,9 +1012,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -867,6 +1022,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,179 +1357,102 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>71</v>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
       <c r="B3" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>224</v>
+      </c>
       <c r="B6" s="6" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>98</v>
-      </c>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
       <c r="B9" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1380,13 +1461,435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="83.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A19:A33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1937,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="23" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1448,7 +1951,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4" t="s">
         <v>138</v>
       </c>
@@ -1460,7 +1963,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="6" t="s">
         <v>141</v>
       </c>
@@ -1472,7 +1975,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="6" t="s">
         <v>139</v>
       </c>
@@ -1484,7 +1987,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
         <v>144</v>
       </c>
@@ -1496,7 +1999,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="10" t="s">
         <v>146</v>
       </c>
@@ -1508,7 +2011,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="10" t="s">
         <v>148</v>
       </c>
@@ -1520,7 +2023,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="10" t="s">
         <v>150</v>
       </c>
@@ -1532,7 +2035,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1546,7 +2049,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1556,7 +2059,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1568,7 +2071,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1580,7 +2083,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -1592,7 +2095,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
@@ -1602,7 +2105,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="6" t="s">
         <v>88</v>
       </c>
@@ -1612,7 +2115,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="6" t="s">
         <v>89</v>
       </c>
@@ -1622,7 +2125,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
@@ -1632,7 +2135,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="6" t="s">
         <v>91</v>
       </c>
@@ -1642,7 +2145,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="6" t="s">
         <v>92</v>
       </c>
@@ -1652,7 +2155,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="6" t="s">
         <v>110</v>
       </c>
@@ -1662,7 +2165,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1676,7 +2179,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1686,7 +2189,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="4" t="s">
         <v>41</v>
       </c>
@@ -1698,7 +2201,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
@@ -1710,7 +2213,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1722,7 +2225,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1734,7 +2237,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
@@ -1746,7 +2249,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
@@ -1758,7 +2261,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1770,7 +2273,7 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1784,7 +2287,7 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="4" t="s">
         <v>46</v>
       </c>
@@ -1796,7 +2299,7 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
@@ -1808,7 +2311,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="6" t="s">
         <v>87</v>
       </c>
@@ -1818,7 +2321,7 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
@@ -1828,7 +2331,7 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="6" t="s">
         <v>89</v>
       </c>
@@ -1838,7 +2341,7 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="6" t="s">
         <v>90</v>
       </c>
@@ -1848,7 +2351,7 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="6" t="s">
         <v>91</v>
       </c>
@@ -1858,7 +2361,7 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="6" t="s">
         <v>94</v>
       </c>
@@ -1867,775 +2370,505 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
-      </c>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="10"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="4"/>
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>19</v>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="4"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>18</v>
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="B45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>4</v>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>20</v>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>21</v>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
+      <c r="B48" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>4</v>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="B49" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>22</v>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="B50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>23</v>
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>4</v>
+      <c r="A52" s="24"/>
+      <c r="B52" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>24</v>
+      <c r="A53" s="24"/>
+      <c r="B53" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>25</v>
+      <c r="A54" s="24"/>
+      <c r="B54" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>16</v>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
+      <c r="B55" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>26</v>
+      <c r="A56" s="25"/>
+      <c r="B56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
+        <v>186</v>
+      </c>
       <c r="B57" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>27</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C57" s="10"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="10" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C59" s="10"/>
+        <v>157</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>158</v>
+      </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="29"/>
       <c r="B60" s="10" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
       <c r="B61" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="10"/>
+        <v>160</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="10"/>
+        <v>162</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="29"/>
       <c r="B63" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C63" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+    <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="29"/>
       <c r="B64" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>31</v>
-      </c>
+    <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="29"/>
       <c r="B65" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C65" s="10"/>
+        <v>167</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>32</v>
+    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="29"/>
+      <c r="B66" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>33</v>
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="29"/>
+      <c r="B67" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>34</v>
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="29"/>
+      <c r="B68" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>35</v>
+      <c r="A69" s="29"/>
+      <c r="B69" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>36</v>
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="29"/>
+      <c r="B70" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>33</v>
+    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="29"/>
+      <c r="B71" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>177</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>26</v>
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="29"/>
+      <c r="B72" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>37</v>
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="29"/>
+      <c r="B73" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>38</v>
+    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="29"/>
+      <c r="B74" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>39</v>
+      <c r="A75" s="29"/>
+      <c r="B75" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>16</v>
+      <c r="A76" s="29"/>
+      <c r="B76" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>63</v>
+    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="29"/>
+      <c r="B77" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>184</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>65</v>
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="29"/>
+      <c r="B78" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>32</v>
+    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="29"/>
+      <c r="B79" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>185</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
-      <c r="B80" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C81" s="10"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
-      <c r="B82" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
-      <c r="B83" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C84" s="10"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-      <c r="B85" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-      <c r="B86" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
-      <c r="B87" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-    </row>
-    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
-      <c r="B88" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-      <c r="B89" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-      <c r="B91" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C91" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
-      <c r="B93" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-    </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-      <c r="B94" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
-      <c r="B95" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
-      <c r="B96" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
-      <c r="B97" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
-      <c r="B98" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-    </row>
-    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
-      <c r="B99" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-    </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
-      <c r="B100" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-    </row>
-    <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
-      <c r="B101" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C101" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-    </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-      <c r="B102" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-    </row>
-    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
-      <c r="B103" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A81:A103"/>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A41:A56"/>
+    <mergeCell ref="A57:A79"/>
     <mergeCell ref="A23:A31"/>
     <mergeCell ref="A11:A22"/>
     <mergeCell ref="A32:A40"/>
-    <mergeCell ref="A41:A64"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A65:A80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="83.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,187 +2891,825 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>114</v>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+        <v>225</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A3:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
merged -r 653:812 branches/CombinedControl
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19320" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
-    <sheet name="Displacement Tests" sheetId="1" r:id="rId2"/>
-    <sheet name="Configuration Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="OM Setup Test" sheetId="3" r:id="rId2"/>
+    <sheet name="No Oil Test" sheetId="1" r:id="rId3"/>
+    <sheet name="Oil Test with Free LBCB(s)" sheetId="6" r:id="rId4"/>
+    <sheet name="Rubber Specimen Test" sheetId="4" r:id="rId5"/>
+    <sheet name="Fake Startup" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="231">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -715,6 +718,138 @@
   </si>
   <si>
     <t>NTCP</t>
+  </si>
+  <si>
+    <t>Operation Manager Configuration Test</t>
+  </si>
+  <si>
+    <t>Select the Edit-&gt;Position menu item</t>
+  </si>
+  <si>
+    <t>The LBCB Position widget should appear</t>
+  </si>
+  <si>
+    <t>Change all of the position  values to unique values  and press OK.  Do this for both LBCBs</t>
+  </si>
+  <si>
+    <t>Reselect Edit-&gt;Position</t>
+  </si>
+  <si>
+    <t>Verify that all of the values are still changed</t>
+  </si>
+  <si>
+    <t>Press OK</t>
+  </si>
+  <si>
+    <t>Restart the LBCB Operation Manager program.  Select Edit-&gt;Position again</t>
+  </si>
+  <si>
+    <t>Verify that all of the values have returned to their original values.</t>
+  </si>
+  <si>
+    <t>Select File-&gt;Save and restart the program</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Position again</t>
+  </si>
+  <si>
+    <t>Verify that the values change when they are supposed to.</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Middle Loop</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Mixed Mode Loop</t>
+  </si>
+  <si>
+    <t>Repeat the test for Edit-&gt;Timing &amp; Logging</t>
+  </si>
+  <si>
+    <t>Repeat the test for the "Auto Balance Control" and "Auto Balance Error Window" in the Autobalance tab</t>
+  </si>
+  <si>
+    <t>Repeat the test for the stiffness matrix, Jacobian Gain, Max Increment, Force Group Priorities, Force Error Range, Stiffness Limits, and Force Control Parameters  in the Mixed Mode tab</t>
+  </si>
+  <si>
+    <t>Repeat this test with Edit-&gt;Limits.  Note There are 16 different displays when selecting a limit set and an LBCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the cartesian force limits to a window that is within the capacity of the rubber specimen.  Move the LBCB a small amount in to translation and two rotation directions.  The translation should be &gt; 0.1 inches.  The rotation should be &gt; .001 radians.  Make sure that none of the translations add tension to the specimen.  </t>
+  </si>
+  <si>
+    <t>Enter ramp times of 2 seconds for all of the ramp entries in the Mixed Mode Window.    Switch the LBCB Operation Manager Window to Mixed Mode.  Set the Jacobian to 0.8 for all DOFs.  Set the max increment to .01 for all translations and .0001 for all rotations.  Set all Force Group Priorities to 5.  Set the Force Error Range to 5 lbs for for the forces and 20 lbs*inches for the moments.  Set the low stiffness limit to 20 and the high limit to 1E+6.  Make sure that all of the force control parameters are set to "No".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the LBCB Operation Manager Window you will see the Convergence display indicating which DOFs are converged as well as which DOF is being controlled.  The stiffness matrix will have updated values for the column associated with the controlling DOF.  The Target display will show for the controlling DOF a displacement that equals the current displacement plus the max increment.  The last step will be slightly less than the max increment.  The force ramp should end with all of the force DOFs converged.  The resulting forces and moments should be 0 +/- the force error </t>
+  </si>
+  <si>
+    <t>The changed DOF will converge to the tighter force error range.</t>
+  </si>
+  <si>
+    <t>You should see a significant increase in force along the directions that are displaced.  Record these force values as force target 1.</t>
+  </si>
+  <si>
+    <t>Make sure that the force DOF with the changed Max Increment shows a displacement in the LBCB Operation Manager Target window that is the current displacement +/- .03.</t>
+  </si>
+  <si>
+    <t>In the Mixed Mode Window set the forces moments which are in the same directions as the displacement DOFs  set earlier to zero.   Press Set Target then Start on the Mixed Mode Window.</t>
+  </si>
+  <si>
+    <t>Enter the forces for target 1 in the Mixed Mode Widget.  Press Set Target and Start</t>
+  </si>
+  <si>
+    <t>The force ramp should stop on a limit fault for the limit that was changed</t>
+  </si>
+  <si>
+    <t>Take a look at which controlling DOF is chosen.  In the previous ramps the moments were chosen first.  In this case the force DOF with the 3 lb force error range should be chosen first.</t>
+  </si>
+  <si>
+    <t>The controlling DOF that is chosen should follow the priorities with the lowest adjusted first.</t>
+  </si>
+  <si>
+    <t>The stiffness matrix will not be updated during this camp.  The controlling DOFs will first adjust all of the DOFs with the lower priority and then it will adjust all of the DOFs in the in the higher party.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the force error range for one of the force DOFs to 3 lbs.  Press Set Target and Start again.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set a limit for one of the target 1 forces to be just under the target 1 magnitude.</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, reset the Max Increment to .01 inches.  Set the Force Control Parameter "Use Force Error Range Ratios" to Yes.  Enter the forces for target 1 and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Use Force Error Range Ratios" to No.  Set the Force Control Paraemter "Use Group Priorities" to Yes.  Enter a different priority for each DOF in the Force Group Priorities display between 0 and 5.  Enter zero for the forces and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Multi Command Update" to Yes.  Enter two  different priorities for the DOF in the Force Group Priorities display.  Enter the target 1 forces and press Set Target and then Start</t>
+  </si>
+  <si>
+    <t>Force Control Test</t>
+  </si>
+  <si>
+    <t>After the ramp is stopped, set the Max increment for one of the force DOFs to .03 inches.  Enter zero for all of the forces in the Mixed Mode Widget.  Press Set Target and Start</t>
+  </si>
+  <si>
+    <t>Turn On Oil</t>
+  </si>
+  <si>
+    <t>This test needs a rigid rubber specimen connected.  The Startup procedure including oil turn on needs to done first.</t>
+  </si>
+  <si>
+    <t>The LBCB(s) should move for 10 seconds to the commanded displacement. The measured displacement should be the same as the commanded displacement when the offset is taken into account.</t>
+  </si>
+  <si>
+    <t>Input a target of displacement Dx within the displacement limits and press "Set Target".  Record the difference between the command displacement and the measured displacment as an offset.</t>
+  </si>
+  <si>
+    <t>Set Rigid Connection to "Yes".  Save the change.</t>
+  </si>
+  <si>
+    <t>Verify that the Rigid Connection is still "Yes".</t>
+  </si>
+  <si>
+    <t>Verify that LBCB2 cannot be selected for the Mixed Mode, and Cartesian Limits pages.</t>
   </si>
 </sst>
 </file>
@@ -810,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -847,6 +982,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -854,9 +1012,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -867,6 +1022,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1169,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,179 +1357,102 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>71</v>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
       <c r="B3" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
       <c r="B5" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>224</v>
+      </c>
       <c r="B6" s="6" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>98</v>
-      </c>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
       <c r="B9" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1380,13 +1461,435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="83.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="29"/>
+      <c r="B22" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="29"/>
+      <c r="B23" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="29"/>
+      <c r="B24" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="29"/>
+      <c r="B29" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="29"/>
+      <c r="B30" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
+      <c r="B31" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
+      <c r="B33" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A19:A33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1937,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="23" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1448,7 +1951,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="4" t="s">
         <v>138</v>
       </c>
@@ -1460,7 +1963,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="6" t="s">
         <v>141</v>
       </c>
@@ -1472,7 +1975,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="6" t="s">
         <v>139</v>
       </c>
@@ -1484,7 +1987,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
         <v>144</v>
       </c>
@@ -1496,7 +1999,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="10" t="s">
         <v>146</v>
       </c>
@@ -1508,7 +2011,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="10" t="s">
         <v>148</v>
       </c>
@@ -1520,7 +2023,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="10" t="s">
         <v>150</v>
       </c>
@@ -1532,7 +2035,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1546,7 +2049,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -1556,7 +2059,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1568,7 +2071,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1580,7 +2083,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -1592,7 +2095,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
@@ -1602,7 +2105,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="6" t="s">
         <v>88</v>
       </c>
@@ -1612,7 +2115,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="6" t="s">
         <v>89</v>
       </c>
@@ -1622,7 +2125,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
@@ -1632,7 +2135,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="6" t="s">
         <v>91</v>
       </c>
@@ -1642,7 +2145,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="6" t="s">
         <v>92</v>
       </c>
@@ -1652,7 +2155,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="6" t="s">
         <v>110</v>
       </c>
@@ -1662,7 +2165,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1676,7 +2179,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1686,7 +2189,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="4" t="s">
         <v>41</v>
       </c>
@@ -1698,7 +2201,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
@@ -1710,7 +2213,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="4" t="s">
         <v>111</v>
       </c>
@@ -1722,7 +2225,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1734,7 +2237,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
@@ -1746,7 +2249,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="4" t="s">
         <v>41</v>
       </c>
@@ -1758,7 +2261,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1770,7 +2273,7 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1784,7 +2287,7 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="4" t="s">
         <v>46</v>
       </c>
@@ -1796,7 +2299,7 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="4" t="s">
         <v>47</v>
       </c>
@@ -1808,7 +2311,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="6" t="s">
         <v>87</v>
       </c>
@@ -1818,7 +2321,7 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
@@ -1828,7 +2331,7 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="6" t="s">
         <v>89</v>
       </c>
@@ -1838,7 +2341,7 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="6" t="s">
         <v>90</v>
       </c>
@@ -1848,7 +2351,7 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="6" t="s">
         <v>91</v>
       </c>
@@ -1858,7 +2361,7 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="6" t="s">
         <v>94</v>
       </c>
@@ -1867,775 +2370,505 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
-      </c>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="10"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="4"/>
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>19</v>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="4"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>18</v>
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="B45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>4</v>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>20</v>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>21</v>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
+      <c r="B48" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>4</v>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="B49" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>22</v>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="B50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>23</v>
+    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>4</v>
+      <c r="A52" s="24"/>
+      <c r="B52" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>24</v>
+      <c r="A53" s="24"/>
+      <c r="B53" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>25</v>
+      <c r="A54" s="24"/>
+      <c r="B54" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>16</v>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
+      <c r="B55" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>26</v>
+      <c r="A56" s="25"/>
+      <c r="B56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
+        <v>186</v>
+      </c>
       <c r="B57" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>27</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C57" s="10"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="29"/>
       <c r="B58" s="10" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="29"/>
       <c r="B59" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C59" s="10"/>
+        <v>157</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>158</v>
+      </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="29"/>
       <c r="B60" s="10" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="29"/>
       <c r="B61" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="10"/>
+        <v>160</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="29"/>
       <c r="B62" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="10"/>
+        <v>162</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="29"/>
       <c r="B63" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C63" s="10"/>
+        <v>50</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+    <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="29"/>
       <c r="B64" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C64" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>31</v>
-      </c>
+    <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="29"/>
       <c r="B65" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C65" s="10"/>
+        <v>167</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>32</v>
+    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="29"/>
+      <c r="B66" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="B67" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>33</v>
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="29"/>
+      <c r="B67" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>34</v>
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="29"/>
+      <c r="B68" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>35</v>
+      <c r="A69" s="29"/>
+      <c r="B69" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>36</v>
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="29"/>
+      <c r="B70" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>33</v>
+    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="29"/>
+      <c r="B71" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>177</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>26</v>
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="29"/>
+      <c r="B72" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>37</v>
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="29"/>
+      <c r="B73" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>38</v>
+    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="29"/>
+      <c r="B74" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>39</v>
+      <c r="A75" s="29"/>
+      <c r="B75" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>16</v>
+      <c r="A76" s="29"/>
+      <c r="B76" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>63</v>
+    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="29"/>
+      <c r="B77" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>184</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>65</v>
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="29"/>
+      <c r="B78" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>161</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>32</v>
+    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="29"/>
+      <c r="B79" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>185</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
-      <c r="B80" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C81" s="10"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
-      <c r="B82" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
-      <c r="B83" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C84" s="10"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-      <c r="B85" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-      <c r="B86" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
-      <c r="B87" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5"/>
-    </row>
-    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
-      <c r="B88" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-      <c r="B89" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-      <c r="B91" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="C91" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
-      <c r="B93" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5"/>
-    </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-      <c r="B94" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
-      <c r="B95" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
-      <c r="B96" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
-      <c r="B97" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
-      <c r="B98" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-    </row>
-    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
-      <c r="B99" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-    </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
-      <c r="B100" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-    </row>
-    <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
-      <c r="B101" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C101" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-    </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-      <c r="B102" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-    </row>
-    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
-      <c r="B103" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A81:A103"/>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A41:A56"/>
+    <mergeCell ref="A57:A79"/>
     <mergeCell ref="A23:A31"/>
     <mergeCell ref="A11:A22"/>
     <mergeCell ref="A32:A40"/>
-    <mergeCell ref="A41:A64"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A65:A80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="83.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58" style="1" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,187 +2891,825 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>114</v>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+        <v>225</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A3:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes to OM Setup and 1/5 scale two box testing
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -850,6 +850,27 @@
   </si>
   <si>
     <t>Verify that LBCB2 cannot be selected for the Mixed Mode, and Cartesian Limits pages.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Do LBCB 1 and LBCB 2 have the same values? i.e. changing one changes the other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBCB 2 cannot be selected for Timing and Logging </t>
+  </si>
+  <si>
+    <t>POP-UP MESSAGE: Selection "Mixed-mode Loop" not recognized!</t>
+  </si>
+  <si>
+    <t>POP-UP MESSAGE: DAQ Receive Channels not configured correctly: ,,,,,,,,,,,LPot3,LPot4,LPot1,LPot2 (swith "Real" to "FAKE!!!")</t>
+  </si>
+  <si>
+    <t>Cannot switch from LBCB 1 to LBCB 2 on Limits tab. And LBCB on Limits tab does not control LBCB on main OM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The values are near what was entered, but not exact (ex. 38 to 41.6667). Cannot switch between LBCB 1 and LBCB 2. Looking at all OM Locations, only "Crane Bay One LBCB" and "Portable LBCB" switch between LBCB 1 and LBCB 2. </t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1536,9 @@
       <c r="C3" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>231</v>
+      </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
@@ -1527,7 +1550,9 @@
       <c r="C4" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
@@ -1539,7 +1564,9 @@
       <c r="C5" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
@@ -1549,7 +1576,9 @@
         <v>119</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
@@ -1561,7 +1590,9 @@
       <c r="C7" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
@@ -1573,7 +1604,9 @@
       <c r="C8" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
@@ -1585,7 +1618,9 @@
       <c r="C9" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
@@ -1597,7 +1632,9 @@
       <c r="C10" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
@@ -1610,8 +1647,12 @@
         <v>127</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
@@ -1621,7 +1662,9 @@
       <c r="C12" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
@@ -1633,7 +1676,9 @@
       <c r="C13" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
@@ -1645,7 +1690,9 @@
       <c r="C14" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
@@ -1657,7 +1704,9 @@
       <c r="C15" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
@@ -1669,9 +1718,13 @@
       <c r="C16" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
@@ -1681,9 +1734,13 @@
       <c r="C17" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
@@ -1693,7 +1750,9 @@
       <c r="C18" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
@@ -1707,9 +1766,13 @@
       <c r="C19" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
@@ -1719,7 +1782,9 @@
       <c r="C20" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
@@ -1729,7 +1794,9 @@
         <v>190</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
@@ -1741,7 +1808,9 @@
       <c r="C22" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
@@ -1751,7 +1820,9 @@
         <v>193</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
@@ -1763,7 +1834,9 @@
       <c r="C24" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
@@ -1773,7 +1846,9 @@
         <v>190</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
@@ -1783,7 +1858,9 @@
         <v>196</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
@@ -1795,7 +1872,9 @@
       <c r="C27" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
@@ -1807,9 +1886,13 @@
       <c r="C28" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="13" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
@@ -1819,7 +1902,9 @@
       <c r="C29" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
@@ -1832,8 +1917,12 @@
         <v>198</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
@@ -1843,7 +1932,9 @@
       <c r="C31" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
@@ -1855,7 +1946,9 @@
       <c r="C32" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
@@ -1867,7 +1960,9 @@
       <c r="C33" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>

</xml_diff>

<commit_message>
merged -r 812:820 branches/CombinedControl
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -850,6 +850,27 @@
   </si>
   <si>
     <t>Verify that LBCB2 cannot be selected for the Mixed Mode, and Cartesian Limits pages.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Do LBCB 1 and LBCB 2 have the same values? i.e. changing one changes the other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBCB 2 cannot be selected for Timing and Logging </t>
+  </si>
+  <si>
+    <t>POP-UP MESSAGE: Selection "Mixed-mode Loop" not recognized!</t>
+  </si>
+  <si>
+    <t>POP-UP MESSAGE: DAQ Receive Channels not configured correctly: ,,,,,,,,,,,LPot3,LPot4,LPot1,LPot2 (swith "Real" to "FAKE!!!")</t>
+  </si>
+  <si>
+    <t>Cannot switch from LBCB 1 to LBCB 2 on Limits tab. And LBCB on Limits tab does not control LBCB on main OM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The values are near what was entered, but not exact (ex. 38 to 41.6667). Cannot switch between LBCB 1 and LBCB 2. Looking at all OM Locations, only "Crane Bay One LBCB" and "Portable LBCB" switch between LBCB 1 and LBCB 2. </t>
   </si>
 </sst>
 </file>
@@ -1463,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1536,9 @@
       <c r="C3" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>231</v>
+      </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
@@ -1527,7 +1550,9 @@
       <c r="C4" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
@@ -1539,7 +1564,9 @@
       <c r="C5" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
@@ -1549,7 +1576,9 @@
         <v>119</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
@@ -1561,7 +1590,9 @@
       <c r="C7" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
@@ -1573,7 +1604,9 @@
       <c r="C8" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
@@ -1585,7 +1618,9 @@
       <c r="C9" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
@@ -1597,7 +1632,9 @@
       <c r="C10" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
@@ -1610,8 +1647,12 @@
         <v>127</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
@@ -1621,7 +1662,9 @@
       <c r="C12" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
@@ -1633,7 +1676,9 @@
       <c r="C13" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
@@ -1645,7 +1690,9 @@
       <c r="C14" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
@@ -1657,7 +1704,9 @@
       <c r="C15" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
@@ -1669,9 +1718,13 @@
       <c r="C16" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="F16" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
@@ -1681,9 +1734,13 @@
       <c r="C17" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
@@ -1693,7 +1750,9 @@
       <c r="C18" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>231</v>
+      </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
@@ -1707,9 +1766,13 @@
       <c r="C19" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
@@ -1719,7 +1782,9 @@
       <c r="C20" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
@@ -1729,7 +1794,9 @@
         <v>190</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
@@ -1741,7 +1808,9 @@
       <c r="C22" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
@@ -1751,7 +1820,9 @@
         <v>193</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
@@ -1763,7 +1834,9 @@
       <c r="C24" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
@@ -1773,7 +1846,9 @@
         <v>190</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
@@ -1783,7 +1858,9 @@
         <v>196</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
@@ -1795,7 +1872,9 @@
       <c r="C27" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
@@ -1807,9 +1886,13 @@
       <c r="C28" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="13" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
@@ -1819,7 +1902,9 @@
       <c r="C29" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
@@ -1832,8 +1917,12 @@
         <v>198</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
@@ -1843,7 +1932,9 @@
       <c r="C31" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
@@ -1855,7 +1946,9 @@
       <c r="C32" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
@@ -1867,7 +1960,9 @@
       <c r="C33" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>231</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added Rigid Connection testing
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="19320" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19320" windowHeight="14370" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="244">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -807,9 +807,6 @@
     <t>The controlling DOF that is chosen should follow the priorities with the lowest adjusted first.</t>
   </si>
   <si>
-    <t>The stiffness matrix will not be updated during this camp.  The controlling DOFs will first adjust all of the DOFs with the lower priority and then it will adjust all of the DOFs in the in the higher party.</t>
-  </si>
-  <si>
     <t>After the ramp is completed, set the force error range for one of the force DOFs to 3 lbs.  Press Set Target and Start again.</t>
   </si>
   <si>
@@ -822,9 +819,6 @@
     <t>After the ramp is completed, set the Force Control Parameter "Use Force Error Range Ratios" to No.  Set the Force Control Paraemter "Use Group Priorities" to Yes.  Enter a different priority for each DOF in the Force Group Priorities display between 0 and 5.  Enter zero for the forces and press Set Target and then Start</t>
   </si>
   <si>
-    <t>After the ramp is completed, set the Force Control Parameter "Multi Command Update" to Yes.  Enter two  different priorities for the DOF in the Force Group Priorities display.  Enter the target 1 forces and press Set Target and then Start</t>
-  </si>
-  <si>
     <t>Force Control Test</t>
   </si>
   <si>
@@ -871,6 +865,30 @@
   </si>
   <si>
     <t xml:space="preserve">The values are near what was entered, but not exact (ex. 38 to 41.6667). Cannot switch between LBCB 1 and LBCB 2. Looking at all OM Locations, only "Crane Bay One LBCB" and "Portable LBCB" switch between LBCB 1 and LBCB 2. </t>
+  </si>
+  <si>
+    <t>Repeat test  by inputing a combintion of DOFs.  For example use Dx and Ry.</t>
+  </si>
+  <si>
+    <t>Repeat test with LBCB 2 if testing with the two box setup</t>
+  </si>
+  <si>
+    <t>Repeat test with the rigid connection button set to 'YES' if testing with the two box setup</t>
+  </si>
+  <si>
+    <t>In this case LBCB 2 becomes a slave to LBCB 1 and only LBCB 1 targets are possible</t>
+  </si>
+  <si>
+    <t>In this case LBCB 2 limits are no longer available and the LBCB 2 movement is defined by the LBCB 1 limits</t>
+  </si>
+  <si>
+    <t>In this case LBCB 2 becomes a slave to LBCB 1 and only LBCB 1 offsets are used for LBCB 2.</t>
+  </si>
+  <si>
+    <t>First,  all of the force DOFs that are not converged will be adjusted one by one to get new stiffness values.  Then the OM will run 3 ramps with updated commands for all non-converged DOFs and no stiffness updates.  After this the stiffness test is repeated</t>
+  </si>
+  <si>
+    <t>After the ramp is completed, set the Force Control Parameter "Multi Command Update" to Yes.  Set Use Group Priorities to "NO".  Set the Stiffness Test Ramp Count to 3.  Enter the target 1 forces and press Set Target and then Start</t>
   </si>
 </sst>
 </file>
@@ -966,7 +984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1026,6 +1044,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1379,7 +1403,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1392,7 +1416,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="6" t="s">
         <v>78</v>
       </c>
@@ -1403,7 +1427,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="6" t="s">
         <v>81</v>
       </c>
@@ -1414,7 +1438,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="6" t="s">
         <v>84</v>
       </c>
@@ -1425,8 +1449,8 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>224</v>
+      <c r="A6" s="25" t="s">
+        <v>222</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>99</v>
@@ -1438,7 +1462,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="6" t="s">
         <v>101</v>
       </c>
@@ -1449,7 +1473,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="6" t="s">
         <v>103</v>
       </c>
@@ -1460,7 +1484,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="6" t="s">
         <v>104</v>
       </c>
@@ -1484,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1517,7 +1541,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>114</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1529,7 +1553,7 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="7" t="s">
         <v>112</v>
       </c>
@@ -1537,13 +1561,13 @@
         <v>113</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="13" t="s">
         <v>116</v>
       </c>
@@ -1551,13 +1575,13 @@
         <v>117</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="13" t="s">
         <v>118</v>
       </c>
@@ -1565,25 +1589,25 @@
         <v>121</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="13" t="s">
         <v>119</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="13" t="s">
         <v>120</v>
       </c>
@@ -1591,13 +1615,13 @@
         <v>124</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="13" t="s">
         <v>122</v>
       </c>
@@ -1605,13 +1629,13 @@
         <v>123</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="13" t="s">
         <v>125</v>
       </c>
@@ -1619,13 +1643,13 @@
         <v>123</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="13" t="s">
         <v>126</v>
       </c>
@@ -1633,13 +1657,13 @@
         <v>128</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="13" t="s">
         <v>129</v>
       </c>
@@ -1648,14 +1672,14 @@
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="13" t="s">
         <v>130</v>
       </c>
@@ -1663,13 +1687,13 @@
         <v>128</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="13" t="s">
         <v>131</v>
       </c>
@@ -1677,13 +1701,13 @@
         <v>128</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="13" t="s">
         <v>132</v>
       </c>
@@ -1691,13 +1715,13 @@
         <v>128</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="13" t="s">
         <v>133</v>
       </c>
@@ -1705,13 +1729,13 @@
         <v>128</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="13" t="s">
         <v>134</v>
       </c>
@@ -1719,45 +1743,45 @@
         <v>128</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>230</v>
-      </c>
       <c r="D17" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="13" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="13" t="s">
         <v>229</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>231</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="31" t="s">
         <v>187</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -1767,15 +1791,15 @@
         <v>97</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="13" t="s">
         <v>188</v>
       </c>
@@ -1783,25 +1807,25 @@
         <v>189</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="13" t="s">
         <v>190</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="13" t="s">
         <v>191</v>
       </c>
@@ -1809,25 +1833,25 @@
         <v>192</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="13" t="s">
         <v>193</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="13" t="s">
         <v>194</v>
       </c>
@@ -1835,37 +1859,37 @@
         <v>195</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="13" t="s">
         <v>190</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="13" t="s">
         <v>196</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="13" t="s">
         <v>197</v>
       </c>
@@ -1873,13 +1897,13 @@
         <v>192</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="13" t="s">
         <v>204</v>
       </c>
@@ -1887,15 +1911,15 @@
         <v>198</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="13" t="s">
         <v>199</v>
       </c>
@@ -1903,13 +1927,13 @@
         <v>198</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="13" t="s">
         <v>200</v>
       </c>
@@ -1918,14 +1942,14 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="13" t="s">
         <v>201</v>
       </c>
@@ -1933,13 +1957,13 @@
         <v>198</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="13" t="s">
         <v>202</v>
       </c>
@@ -1947,13 +1971,13 @@
         <v>198</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="13" t="s">
         <v>203</v>
       </c>
@@ -1961,7 +1985,7 @@
         <v>198</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1981,10 +2005,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,7 +2056,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2046,7 +2070,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="4" t="s">
         <v>138</v>
       </c>
@@ -2058,7 +2082,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="6" t="s">
         <v>141</v>
       </c>
@@ -2070,7 +2094,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="6" t="s">
         <v>139</v>
       </c>
@@ -2082,7 +2106,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="6" t="s">
         <v>144</v>
       </c>
@@ -2094,7 +2118,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="10" t="s">
         <v>146</v>
       </c>
@@ -2106,7 +2130,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="10" t="s">
         <v>148</v>
       </c>
@@ -2118,7 +2142,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="10" t="s">
         <v>150</v>
       </c>
@@ -2130,7 +2154,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2144,7 +2168,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
@@ -2154,7 +2178,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
@@ -2166,7 +2190,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
@@ -2178,7 +2202,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2190,7 +2214,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
@@ -2200,7 +2224,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="6" t="s">
         <v>88</v>
       </c>
@@ -2210,7 +2234,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="6" t="s">
         <v>89</v>
       </c>
@@ -2220,7 +2244,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="6" t="s">
         <v>90</v>
       </c>
@@ -2230,7 +2254,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="6" t="s">
         <v>91</v>
       </c>
@@ -2239,196 +2263,198 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
       <c r="B21" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="6"/>
+        <v>236</v>
+      </c>
+      <c r="C21" s="24"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="6"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="C22" s="24"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
+      <c r="A23" s="26"/>
+      <c r="B23" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="4"/>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="6"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>8</v>
+      </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="4" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="31"/>
       <c r="B29" s="4" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
       <c r="B30" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
       <c r="B31" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>14</v>
-      </c>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="4" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
       <c r="B33" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
+      <c r="A34" s="25" t="s">
+        <v>14</v>
+      </c>
       <c r="B34" s="4" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="6"/>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="6"/>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="5"/>
@@ -2436,9 +2462,9 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="5"/>
@@ -2446,19 +2472,19 @@
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
       <c r="B40" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="5"/>
@@ -2466,79 +2492,73 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="10"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="6"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
       <c r="B42" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C42" s="6"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A43" s="23"/>
+      <c r="B43" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="24"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>34</v>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>240</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
-    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>35</v>
-      </c>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="10"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
       <c r="B46" s="6" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="6" t="s">
         <v>56</v>
       </c>
@@ -2550,295 +2570,295 @@
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
       <c r="B49" s="6" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="26"/>
       <c r="B50" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="26"/>
       <c r="B51" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
       <c r="B52" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="24"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
       <c r="B53" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="26"/>
       <c r="B54" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="24"/>
+    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
       <c r="B55" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="26"/>
       <c r="B56" s="6" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C57" s="10"/>
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="26"/>
+      <c r="B57" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
-      <c r="B58" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>156</v>
+      <c r="A58" s="26"/>
+      <c r="B58" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
-      <c r="B59" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>158</v>
+      <c r="A59" s="26"/>
+      <c r="B59" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
-    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
-      <c r="B60" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C60" s="10"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="27"/>
+      <c r="B60" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
     </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="31" t="s">
+        <v>186</v>
+      </c>
       <c r="B61" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>161</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C61" s="10"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="29"/>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
       <c r="B63" s="10" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>166</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C64" s="10"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="29"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="10" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
       <c r="B66" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="29"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="10" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="31"/>
       <c r="B71" s="10" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="10" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>161</v>
@@ -2848,21 +2868,21 @@
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="10" t="s">
         <v>173</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
+      <c r="A74" s="31"/>
       <c r="B74" s="10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>161</v>
@@ -2872,21 +2892,21 @@
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
+      <c r="A75" s="31"/>
       <c r="B75" s="10" t="s">
         <v>173</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="31"/>
       <c r="B76" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>161</v>
@@ -2895,22 +2915,22 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="31"/>
       <c r="B77" s="10" t="s">
         <v>173</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="29"/>
+      <c r="A78" s="31"/>
       <c r="B78" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>161</v>
@@ -2920,25 +2940,73 @@
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A79" s="29"/>
+      <c r="A79" s="31"/>
       <c r="B79" s="10" t="s">
         <v>173</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
+    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="31"/>
+      <c r="B80" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="31"/>
+      <c r="B81" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="31"/>
+      <c r="B82" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A83" s="31"/>
+      <c r="B83" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A41:A56"/>
-    <mergeCell ref="A57:A79"/>
-    <mergeCell ref="A23:A31"/>
-    <mergeCell ref="A11:A22"/>
-    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="A45:A60"/>
+    <mergeCell ref="A61:A83"/>
+    <mergeCell ref="A25:A33"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="A34:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2950,10 +3018,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,11 +3055,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>4</v>
@@ -3001,7 +3069,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="18" t="s">
         <v>40</v>
       </c>
@@ -3011,19 +3079,19 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="18" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="18" t="s">
         <v>42</v>
       </c>
@@ -3035,7 +3103,7 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="18" t="s">
         <v>41</v>
       </c>
@@ -3047,7 +3115,7 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="18" t="s">
         <v>87</v>
       </c>
@@ -3057,7 +3125,7 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="18" t="s">
         <v>88</v>
       </c>
@@ -3067,7 +3135,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="18" t="s">
         <v>89</v>
       </c>
@@ -3077,7 +3145,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="18" t="s">
         <v>90</v>
       </c>
@@ -3087,7 +3155,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="18" t="s">
         <v>91</v>
       </c>
@@ -3097,7 +3165,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="18" t="s">
         <v>92</v>
       </c>
@@ -3107,7 +3175,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="18" t="s">
         <v>110</v>
       </c>
@@ -3116,8 +3184,8 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -3131,7 +3199,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="18" t="s">
         <v>40</v>
       </c>
@@ -3141,7 +3209,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="18" t="s">
         <v>41</v>
       </c>
@@ -3153,7 +3221,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="18" t="s">
         <v>48</v>
       </c>
@@ -3163,7 +3231,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="18" t="s">
         <v>49</v>
       </c>
@@ -3175,7 +3243,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="18" t="s">
         <v>68</v>
       </c>
@@ -3187,7 +3255,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="18" t="s">
         <v>50</v>
       </c>
@@ -3199,7 +3267,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="18" t="s">
         <v>51</v>
       </c>
@@ -3211,7 +3279,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="18" t="s">
         <v>69</v>
       </c>
@@ -3223,7 +3291,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="18" t="s">
         <v>46</v>
       </c>
@@ -3235,7 +3303,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="18" t="s">
         <v>52</v>
       </c>
@@ -3247,7 +3315,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="18" t="s">
         <v>70</v>
       </c>
@@ -3259,7 +3327,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="18" t="s">
         <v>44</v>
       </c>
@@ -3271,7 +3339,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="18" t="s">
         <v>51</v>
       </c>
@@ -3283,7 +3351,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="18" t="s">
         <v>53</v>
       </c>
@@ -3295,7 +3363,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="18" t="s">
         <v>54</v>
       </c>
@@ -3307,7 +3375,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="18" t="s">
         <v>44</v>
       </c>
@@ -3319,7 +3387,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="18" t="s">
         <v>55</v>
       </c>
@@ -3331,7 +3399,7 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="18" t="s">
         <v>87</v>
       </c>
@@ -3341,7 +3409,7 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="18" t="s">
         <v>88</v>
       </c>
@@ -3351,7 +3419,7 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="18" t="s">
         <v>89</v>
       </c>
@@ -3361,7 +3429,7 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="18" t="s">
         <v>90</v>
       </c>
@@ -3371,7 +3439,7 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="18" t="s">
         <v>91</v>
       </c>
@@ -3381,7 +3449,7 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="18" t="s">
         <v>92</v>
       </c>
@@ -3390,10 +3458,32 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="C38" s="24"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="27"/>
+      <c r="B39" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A37"/>
+    <mergeCell ref="A14:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3404,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,7 +3531,7 @@
         <v>108</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>107</v>
@@ -3451,8 +3541,8 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>222</v>
+      <c r="A3" s="25" t="s">
+        <v>220</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>205</v>
@@ -3465,7 +3555,7 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="1" t="s">
         <v>206</v>
       </c>
@@ -3475,7 +3565,7 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="16" t="s">
         <v>211</v>
       </c>
@@ -3487,9 +3577,9 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>208</v>
@@ -3499,16 +3589,16 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="16" t="s">
         <v>212</v>
       </c>
@@ -3520,9 +3610,9 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>210</v>
@@ -3532,9 +3622,9 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>214</v>
@@ -3544,9 +3634,9 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>215</v>
@@ -3555,13 +3645,13 @@
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
       <c r="B12" s="16" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -3633,7 +3723,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -3646,7 +3736,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="18" t="s">
         <v>74</v>
       </c>
@@ -3657,7 +3747,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="18" t="s">
         <v>76</v>
       </c>
@@ -3668,7 +3758,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="18" t="s">
         <v>79</v>
       </c>
@@ -3679,7 +3769,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="18" t="s">
         <v>78</v>
       </c>
@@ -3690,7 +3780,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="18" t="s">
         <v>81</v>
       </c>
@@ -3701,7 +3791,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="18" t="s">
         <v>84</v>
       </c>
@@ -3712,7 +3802,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="25" t="s">
         <v>98</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -3725,7 +3815,7 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="18" t="s">
         <v>78</v>
       </c>
@@ -3736,7 +3826,7 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="18" t="s">
         <v>81</v>
       </c>
@@ -3747,7 +3837,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="18" t="s">
         <v>84</v>
       </c>
@@ -3758,7 +3848,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="18" t="s">
         <v>99</v>
       </c>
@@ -3769,7 +3859,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="18" t="s">
         <v>101</v>
       </c>
@@ -3780,7 +3870,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="18" t="s">
         <v>103</v>
       </c>
@@ -3791,7 +3881,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="18" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
New force offset test
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="19320" windowHeight="13620" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19320" windowHeight="9210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Startup" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="281">
   <si>
     <t>Manual input complete step</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Press Decline</t>
   </si>
   <si>
-    <t>Press stop.</t>
-  </si>
-  <si>
     <t>Open the Limits display and check the Local limit for a DOF.  Record the global limit also.  Close the limits display and set a target that is just beyond the largest target in the input file.</t>
   </si>
   <si>
@@ -462,9 +459,6 @@
     <t>All moments for all LBCBs should be displayed in the Targets window with their current value</t>
   </si>
   <si>
-    <t>Press Load and select an input file for each LBCB  being tested that is within the limits of the DOFs being controlled for the first few steps.  Later on in the  test there needs to be a target that exceeds a limit.</t>
-  </si>
-  <si>
     <t>Select Input File Mode</t>
   </si>
   <si>
@@ -501,13 +495,7 @@
     <t>Press the Decline button</t>
   </si>
   <si>
-    <t>The command window should display "ABORTING PROPOSE COMMAND".  The script should send another step with Dx = 1.  The Accept button should be blinking</t>
-  </si>
-  <si>
     <t>Press the Accept button and then the Stop button</t>
-  </si>
-  <si>
-    <t>The command window should display "ABORTING EXECUTE COMMAND".  The script should send another step with Dx = -1.  The Accept button should be blinking.</t>
   </si>
   <si>
     <t>Press "Disconnect NTCP" and type &lt;CTRL&gt; C in the command window</t>
@@ -828,9 +816,6 @@
     <t>Verify that LBCB2 cannot be selected for the Mixed Mode, and Cartesian Limits pages.</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Do LBCB 1 and LBCB 2 have the same values? i.e. changing one changes the other</t>
   </si>
   <si>
@@ -864,186 +849,16 @@
     <t>In this case LBCB 2 limits are no longer available and the LBCB 2 movement is defined by the LBCB 1 limits</t>
   </si>
   <si>
-    <t>In this case LBCB 2 becomes a slave to LBCB 1 and only LBCB 1 offsets are used for LBCB 2.</t>
-  </si>
-  <si>
     <t>First,  all of the force DOFs that are not converged will be adjusted one by one to get new stiffness values.  Then the OM will run 3 ramps with updated commands for all non-converged DOFs and no stiffness updates.  After this the stiffness test is repeated</t>
   </si>
   <si>
     <t>After the ramp is completed, set the Force Control Parameter "Multi Command Update" to Yes.  Set Use Group Priorities to "NO".  Set the Stiffness Test Ramp Count to 3.  Enter the target 1 forces and press Set Target and then Start</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Set 'Rigid Connection' to 'No' then 'Apply' reset targets to zero (to regain access to all grayed out targets) and apply a displacement.  After starting, LBCB 2 will jump back to the previously input displacement in the rigid configuration.</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>Fault message on actuator clears automatically after ~5 seconds.  Displacement fault(s) stays green.</t>
-  </si>
-  <si>
-    <t>Input file "Large Scale 6 DOF Large Steps" executed for LBCB1 and LBCB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due to first failure, I tried switching propose-&gt;Auto and then Execute-&gt;Auto.  After pressing 'Auto' on 'Execute' the step starts automatically.  Multiple targets were then executed correctly. </t>
-  </si>
-  <si>
-    <t>Indicate input file to use.</t>
-  </si>
-  <si>
-    <r>
-      <t>Switch Propose:Manual to Auto and Press Run  (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Press run)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Switch Execute:Manual to Auto and Press Start (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Switch Propose:Manual to Auto and Execute:Manual to Auto)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Pause/Running should be running.  The start button should start blinking.  (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The accept button should start blinking.)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Press Run </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Press Run, Switch Propose:Manual to Auto and Execute:Manual to Auto)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Press Pause </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Press Stop)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mixed Mode State display should iterate through 'Ramp',  </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Stab', and 'Hold'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(and then 'Stab' and 'Hold' for Dispacement and for Force)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Command at the end of the ramp should be the same as the target.   The MM State should be 'Idle' at the end of the ramp.</t>
-    </r>
-  </si>
-  <si>
-    <t>After imposing "rigid connection" to "Yes", for all target patterns when LBCB2 is displayed, hitting "Set Target" grays out the LBCB2 values and gives the error message "Target Type Detected".  "Set Target" must be hit again to execute the targets.  Subsequent tests do not produce the error, only initially.</t>
-  </si>
-  <si>
     <t>Press 'Set Target'</t>
   </si>
   <si>
     <t>'Start' button should blink.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Target should consist of all 6 displacement DOFs set to zero.  </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Start' button should blink.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1075,23 +890,146 @@
     <t>Press "Connect NTCP" to restart the widget for each of the following tests</t>
   </si>
   <si>
-    <t>After declining, the command window reads "aborting propose command" and sends another step of dx = -1</t>
-  </si>
-  <si>
-    <t>There is no 'Pause' button.  If 'Stop' is pressed during the ramp, then pressing 'Run' to restart the process causes the target to be updated to next step ignoring the current step.  There is currently no way to 'Pause' the test.</t>
-  </si>
-  <si>
-    <t>Limits set to be exceeded during the test are Dz for LBCB1 and Rz for LBCB2</t>
-  </si>
-  <si>
-    <t>The target does not change and the step continues correctly.</t>
+    <t>Mixed Mode State display should iterate through 'Ramp' and then 'Stab' and 'Hold' for Displacement and for Force. The command at the end of the ramp should be the same as the target.   The MM State should be 'Idle' at the end of the ramp.</t>
+  </si>
+  <si>
+    <t>Target should consist of all 6 displacement DOFs set to zero.</t>
+  </si>
+  <si>
+    <t>The fault light should turn green.  The fault message should clear after about 5 seconds.  The command for the faulted DOF should not change significantly.</t>
+  </si>
+  <si>
+    <t>Repeat test with the rigid connection button set to 'YES' if testing with the two box setup.  This needs to be done in OM Setup.  After imposing "rigid connection" to "Yes", for all target patterns when LBCB2 is displayed, hitting "Set Target" grays out the LBCB2 values and gives the error message "Target Type Detected".  "Set Target" must be hit again to execute the targets.  Subsequent tests do not produce the error, only initially.</t>
+  </si>
+  <si>
+    <t>Press Load and select an input file for each LBCB  being tested that is within the limits of the DOFs being controlled for the first few steps.  Later on in the  test there needs to be a target that exceeds a limit.  For Example,  if testing on the large scale system,  select the file  "Large Scale 6 DOF Large Steps" for each LBCB.  For this file limits set to be exceeded during the test can be Dz for LBCB1 and Rz for LBCB2</t>
+  </si>
+  <si>
+    <t>Press Stop.</t>
+  </si>
+  <si>
+    <t>Switch Propose:Manual to Auto and Execute:Manual to Auto when the Accept and Start  buttons are blinking.</t>
+  </si>
+  <si>
+    <t>Press Run.  Switch Propose:Manual to Auto and Execute:Manual to Auto</t>
+  </si>
+  <si>
+    <t>Pause/Running should be running.  The accept button should start blinking.</t>
+  </si>
+  <si>
+    <t>Press Stop</t>
+  </si>
+  <si>
+    <t>The command window should display "ABORTING PROPOSE COMMAND".  The script will immediately send another step with Dx = 1.  The Accept button should be blinking.  During an actual test the LbcbPlugin will pause running when it receives a "decline" response.</t>
+  </si>
+  <si>
+    <t>The command window should display "ABORTING EXECUTE COMMAND".  The script will immediately send another step with Dx = -1.  The Accept button should be blinking. During an actual test the LbcbPlugin will pause running when it receives a "stop" response.</t>
+  </si>
+  <si>
+    <t>Force Control With Offsets Test</t>
+  </si>
+  <si>
+    <t>The forces will be close to zero.  However there will be some residual displacement readings due to deformations in the rubber.</t>
+  </si>
+  <si>
+    <t>Open the Offsets widget and set the displacement command offsets and displacement offsets to the current position using the "Execute" feature.</t>
+  </si>
+  <si>
+    <t>Toggle the Global button to Local and back several times and not how all of the displacements change in both the LBCB Operations Manager window and the Mixed Mode window.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The displacements in the Mixed Mode widget and the LBCB Operations Manager should read zero when the "Global" button is set to "Local".  This is true for both cartesian and actuator space displacement commands and readings. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both displacements and forces in the Mixed Mode widget and the LBCB Operations Manager should read zero when the "Global" button is set to "Local".  This is true for both cartesian and actuator space displacement commands and readings. </t>
+  </si>
+  <si>
+    <t>In the Offsets Widget,  create a new force offset at the current position.   Call this offset "Test1"</t>
+  </si>
+  <si>
+    <t>Set the force tag to "Test1" and toggle the Global button to Local and back several times and not how all of the numbers change in both the LBCB Operations Manager window and the Mixed Mode window.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch back to Local.  In the Mixed Mode window select Dx,Dz,Rz, Fz, and My targets.  Toggle the Local button to Global. </t>
+  </si>
+  <si>
+    <t>All of the targets should be set to the offset values with the signs reversed.</t>
+  </si>
+  <si>
+    <t>Switch back to Local.  Clear the targets.  Apply axial force to the specimen by setting Fz to between 10 and 20 pounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After the force command is finished,  Fz should read whatever was targeted. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open the Offset widget and set another Force offset with the tag "Test2". </t>
+  </si>
+  <si>
+    <t>Switch the Force tag on the Mixed Mode widget to "Test 2"</t>
+  </si>
+  <si>
+    <t>Fz should be zero when in Local</t>
+  </si>
+  <si>
+    <t>Shut down the oil and restart the OM</t>
+  </si>
+  <si>
+    <t>In the Offsets window when the Force offsets are selected,  The force tag selector should contain &lt;None&gt;, Test, and Test2</t>
+  </si>
+  <si>
+    <t>Switch the Force tag on the Mixed Mode widget to "Test 1".  Switch to Local</t>
+  </si>
+  <si>
+    <t>In the Mixed Mode window,  Select the "Reset to Zero" pattern and execute this target.</t>
+  </si>
+  <si>
+    <t>After the command is finished all forces and displacements should be zero.</t>
+  </si>
+  <si>
+    <t>Switch the force tag in the Mixed Mode window to "Test 2"</t>
+  </si>
+  <si>
+    <t>The Fz command should read -10 to -20 pounds depending on what axial force you applied earlier</t>
+  </si>
+  <si>
+    <t>In this case the offset widget will compute offsets for the combined LBCBs in addition to the separate boxes.</t>
+  </si>
+  <si>
+    <t>With the OM shut down and the oil off,  use a tape measure to measure the difference between the top center of the rubber specimen and the center of the platten.  Start the OM setup program and enter these measurements as the motion center for LBCB 1.  Make sure that you account for the axis orientation of the LBCB</t>
+  </si>
+  <si>
+    <t>Since the rubber specimen is already connected,  this relative tape measure is sufficient to determine the motion center.  However for the outside tests, the motion center needs to be measured before connection so that the krypton alignment is referenced to this control point.  The cartesian position of the LBCB needs to be include in the calculation of the motion center because of this.</t>
+  </si>
+  <si>
+    <t>Shut down the oil and start up OM Setup. Set the motion center to all zeros.  Restart the OM, autobalance and turn on the oil.</t>
+  </si>
+  <si>
+    <t>Use manual force commands to minimize all of the forces to as close to zero as possible.  Take a snapshot after the minimization is completed and label it Run 1</t>
+  </si>
+  <si>
+    <t>After autobalancing,  open the Offsets window and load the Offsets from Run 1.</t>
+  </si>
+  <si>
+    <t>Load the offsets from Run 1</t>
+  </si>
+  <si>
+    <t>All of the commands and displacments in actuator space should be zero.  The displacements and forces in cartesian space will not necessarily be zero because of the change in geometry due to the new motion center.</t>
+  </si>
+  <si>
+    <t>Take another snapshot and call it Run 2.</t>
+  </si>
+  <si>
+    <t>Compare the actuator displacments and forces between run 1 and run 2</t>
+  </si>
+  <si>
+    <t>All of the values will be the same.  The cartesian values will be different due to the change in motion center.  For extra credit you could do a force equilibrium analysis with the actuator forces to determine if the change in cartesian values are correct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1115,33 +1053,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -1208,7 +1126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1264,13 +1182,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1295,30 +1222,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1615,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,9 +1636,11 @@
     <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1644,98 +1656,112 @@
       <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>93</v>
+      <c r="F1" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="28">
+        <v>40989</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
       <c r="B3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
       <c r="B5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>216</v>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>212</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="B8" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
       <c r="B9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1749,10 +1775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,9 +1787,10 @@
     <col min="2" max="2" width="43.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" style="11" customWidth="1"/>
     <col min="6" max="6" width="83.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1780,456 +1807,397 @@
         <v>29</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="28">
+        <v>40989</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
       <c r="B3" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>223</v>
-      </c>
+      <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
       <c r="B4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>223</v>
-      </c>
+      <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
       <c r="B6" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
-        <v>223</v>
-      </c>
+      <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
       <c r="B7" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
       <c r="B8" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>223</v>
-      </c>
+      <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
       <c r="B9" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
       <c r="B10" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
       <c r="B11" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C12" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>223</v>
-      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
       <c r="B13" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
       <c r="B14" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
       <c r="B15" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
       <c r="B16" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>223</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>181</v>
+      <c r="A19" s="36" t="s">
+        <v>177</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="13" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="13" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="13" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="13" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="E30" s="5"/>
       <c r="F30" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="13" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
@@ -2238,6 +2206,16 @@
     <mergeCell ref="A2:A18"/>
     <mergeCell ref="A19:A33"/>
   </mergeCells>
+  <conditionalFormatting sqref="D2:D33">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="2">
+      <formula>LEN(TRIM(D2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="1">
+      <formula>LEN(TRIM(E2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2248,10 +2226,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E85" sqref="E2:E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2262,9 +2240,10 @@
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2281,1168 +2260,985 @@
         <v>29</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G1" s="28">
+        <v>40989</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>238</v>
-      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>132</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>131</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>240</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
       <c r="B5" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>240</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
       <c r="B6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="B8" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
       <c r="B9" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
       <c r="B10" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="33"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
       <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="C13" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
       <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
       <c r="B15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
       <c r="B16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="5" t="s">
-        <v>240</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="A22" s="31"/>
+      <c r="B22" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
       <c r="B23" s="1" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>240</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="37" t="s">
-        <v>251</v>
-      </c>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="5" t="s">
-        <v>240</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="32" t="s">
-        <v>239</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="C31" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>253</v>
+      <c r="A32" s="36"/>
+      <c r="B32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>233</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="30" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
       <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="6"/>
-      <c r="D38" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="6"/>
-      <c r="D39" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="6"/>
-      <c r="D40" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="6"/>
-      <c r="D41" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="6"/>
-      <c r="D42" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="32"/>
       <c r="B43" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43" s="6"/>
-      <c r="D43" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="32" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="A44" s="21"/>
+      <c r="B44" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="31" t="s">
         <v>30</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5"/>
-      <c r="F46" s="32" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+    </row>
+    <row r="47" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
       <c r="B47" s="6" t="s">
-        <v>147</v>
+        <v>240</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="5" t="s">
-        <v>259</v>
-      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="31"/>
       <c r="B52" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="31"/>
       <c r="B53" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
+      <c r="A54" s="31"/>
       <c r="B54" s="6" t="s">
-        <v>57</v>
+        <v>241</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="C55" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36" t="s">
-        <v>223</v>
-      </c>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>244</v>
+      </c>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
-      <c r="B56" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="C56" s="35" t="s">
+      <c r="A56" s="31"/>
+      <c r="B56" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36" t="s">
-        <v>223</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>243</v>
-      </c>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="38" t="s">
-        <v>248</v>
+      <c r="A58" s="31"/>
+      <c r="B58" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="C58" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
+      <c r="B59" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
-      <c r="B59" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
-      <c r="B60" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="C60" s="35" t="s">
+      <c r="A60" s="31"/>
+      <c r="B60" t="s">
+        <v>245</v>
+      </c>
+      <c r="C60" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D60" s="36"/>
-      <c r="E60" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="F60" s="32" t="s">
-        <v>258</v>
-      </c>
+      <c r="D60" s="25"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
+      <c r="A61" s="32"/>
       <c r="B61" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="31" t="s">
-        <v>180</v>
+      <c r="A62" s="36" t="s">
+        <v>176</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C62" s="10"/>
-      <c r="D62" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
+      <c r="A63" s="36"/>
       <c r="B63" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
+      <c r="A64" s="36"/>
       <c r="B64" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
+      <c r="A65" s="36"/>
       <c r="B65" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C65" s="10"/>
-      <c r="D65" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="31"/>
+      <c r="A66" s="36"/>
       <c r="B66" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
+      <c r="A67" s="36"/>
       <c r="B67" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
+      <c r="A68" s="36"/>
       <c r="B68" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C68" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="C68" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="36"/>
       <c r="B69" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>160</v>
+        <v>246</v>
       </c>
       <c r="D69" s="5"/>
-      <c r="E69" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="36"/>
       <c r="B70" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+      <c r="A71" s="36"/>
       <c r="B71" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+      <c r="A72" s="36"/>
       <c r="B72" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
-      <c r="B73" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="C73" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="A73" s="36"/>
+      <c r="B73" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
+      <c r="A74" s="36"/>
       <c r="B74" s="10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
+        <v>154</v>
+      </c>
+      <c r="D74" s="5"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="25"/>
     </row>
     <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="31"/>
+      <c r="A75" s="36"/>
       <c r="B75" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="31"/>
+      <c r="A76" s="36"/>
       <c r="B76" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="31"/>
+      <c r="A77" s="36"/>
       <c r="B77" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C77" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
+      <c r="A78" s="36"/>
       <c r="B78" s="10" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
+      <c r="A79" s="36"/>
       <c r="B79" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
+      <c r="A80" s="36"/>
       <c r="B80" s="10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="31"/>
+      <c r="A81" s="36"/>
       <c r="B81" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
     <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A82" s="31"/>
+      <c r="A82" s="36"/>
       <c r="B82" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A83" s="31"/>
+      <c r="A83" s="36"/>
       <c r="B83" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="31"/>
+      <c r="A84" s="36"/>
       <c r="B84" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D84" s="5"/>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A85" s="31"/>
+      <c r="A85" s="36"/>
       <c r="B85" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>223</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
     </row>
@@ -3455,6 +3251,16 @@
     <mergeCell ref="A11:A24"/>
     <mergeCell ref="A35:A43"/>
   </mergeCells>
+  <conditionalFormatting sqref="D2:D85">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="2">
+      <formula>LEN(TRIM(D2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E85">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(E2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -3465,10 +3271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,9 +3285,10 @@
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3498,15 +3305,18 @@
         <v>29</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="28">
+        <v>40989</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>4</v>
@@ -3515,8 +3325,8 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
       <c r="B3" s="18" t="s">
         <v>38</v>
       </c>
@@ -3525,20 +3335,20 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
       <c r="B5" s="18" t="s">
         <v>40</v>
       </c>
@@ -3549,94 +3359,94 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
       <c r="B6" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="B8" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
       <c r="B9" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
       <c r="B10" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
       <c r="B11" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
       <c r="B12" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
       <c r="B13" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>4</v>
@@ -3645,8 +3455,8 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
       <c r="B15" s="18" t="s">
         <v>38</v>
       </c>
@@ -3655,8 +3465,8 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
       <c r="B16" s="18" t="s">
         <v>39</v>
       </c>
@@ -3668,7 +3478,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="18" t="s">
         <v>46</v>
       </c>
@@ -3678,7 +3488,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="18" t="s">
         <v>47</v>
       </c>
@@ -3690,9 +3500,9 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>4</v>
@@ -3702,7 +3512,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="18" t="s">
         <v>48</v>
       </c>
@@ -3714,7 +3524,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="18" t="s">
         <v>49</v>
       </c>
@@ -3726,9 +3536,9 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>4</v>
@@ -3738,7 +3548,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="18" t="s">
         <v>44</v>
       </c>
@@ -3750,7 +3560,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="18" t="s">
         <v>50</v>
       </c>
@@ -3762,9 +3572,9 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>4</v>
@@ -3774,7 +3584,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="18" t="s">
         <v>42</v>
       </c>
@@ -3786,7 +3596,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="18" t="s">
         <v>49</v>
       </c>
@@ -3798,7 +3608,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="18" t="s">
         <v>51</v>
       </c>
@@ -3810,7 +3620,7 @@
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="18" t="s">
         <v>52</v>
       </c>
@@ -3822,7 +3632,7 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="18" t="s">
         <v>42</v>
       </c>
@@ -3834,7 +3644,7 @@
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="18" t="s">
         <v>53</v>
       </c>
@@ -3846,9 +3656,9 @@
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="5"/>
@@ -3856,9 +3666,9 @@
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="5"/>
@@ -3866,9 +3676,9 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="5"/>
@@ -3876,9 +3686,9 @@
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="5"/>
@@ -3886,9 +3696,9 @@
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="5"/>
@@ -3896,9 +3706,9 @@
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="5"/>
@@ -3906,22 +3716,22 @@
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="C38" s="24"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" s="22"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>235</v>
+      <c r="A39" s="32"/>
+      <c r="B39" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>270</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -3932,6 +3742,16 @@
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A39"/>
   </mergeCells>
+  <conditionalFormatting sqref="D2:D39">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="2">
+      <formula>LEN(TRIM(D2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E39">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(E2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -3939,10 +3759,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,10 +3770,11 @@
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="72" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3970,168 +3791,394 @@
         <v>29</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G1" s="28">
+        <v>41003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>214</v>
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>199</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>203</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
       <c r="B5" s="16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
       <c r="B6" s="16" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="B8" s="16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
       <c r="B9" s="16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
       <c r="B10" s="16" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
       <c r="B11" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
       <c r="B12" s="16" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="37"/>
+      <c r="B16" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
+      <c r="B18" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
+      <c r="B24" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
+      <c r="B26" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
+      <c r="B27" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="37"/>
+      <c r="B28" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="37"/>
+      <c r="B29" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="37"/>
+      <c r="B30" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="37"/>
+      <c r="B31" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="37"/>
+      <c r="B32" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A33"/>
   </mergeCells>
+  <conditionalFormatting sqref="D2:D33">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="2">
+      <formula>LEN(TRIM(D2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E33">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="1">
+      <formula>LEN(TRIM(E2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4139,10 +4186,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,9 +4197,10 @@
     <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="60.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -4168,172 +4216,175 @@
       <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="F1" s="28">
+        <v>40989</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
       <c r="B3" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>72</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
       <c r="B5" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
       <c r="B6" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
       <c r="B8" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>93</v>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>91</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>92</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
       <c r="B10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
       <c r="B11" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
       <c r="B12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
       <c r="B13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>94</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>95</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
       <c r="B14" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>96</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>97</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
       <c r="B15" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+    <row r="16" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
       <c r="B16" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>99</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>100</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>

</xml_diff>